<commit_message>
Added 0210 and 0211 - TICC-171
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Participant identifier schemes v7.5.xlsx
+++ b/work-in-progress/Peppol Code Lists - Participant identifier schemes v7.5.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6037DC-A7DC-4AA7-AFD9-885CE850B9AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472BF571-7439-4E9F-BAAE-8616315DE727}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$M$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$M$87</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
 </workbook>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="490">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -1688,6 +1688,56 @@
   </si>
   <si>
     <t>414541000099999325412345678901234567890</t>
+  </si>
+  <si>
+    <t>0210</t>
+  </si>
+  <si>
+    <t>0211</t>
+  </si>
+  <si>
+    <t>CODICE FISCALE</t>
+  </si>
+  <si>
+    <t>Agenzia delle Entrate</t>
+  </si>
+  <si>
+    <t>The code is 16 alphanumeric digits for natural persons or 11 numeric digits for legal persons.
+The code is 16 alphanumeric digits for natural persons, with this structure:
+3 digits - Surname according to specific rules
+3 digits - Name according to specific rules
+2 digits - Last two digits of year of birth
+1 digit - Month of birth according to a specific conversion table
+2 digits - Day of birth and gender
+4 digits - Place of birth in a “Belfiore” code
+1 digit - CIN – Control Internal Number
+The code is 11 numeric digits for legal persons, with this structure:
+7 digits - Progressive number
+3 digits - Revenue Office ID
+1 digit - check
+Last digit for natural persons - CIN - Control Internal Number
+Last digit for legal persons - Check</t>
+  </si>
+  <si>
+    <t>Character Repertoire : A to Z (upper case) and 0 to 9</t>
+  </si>
+  <si>
+    <t>Codice fiscale is the Italian tax identification number and is the code that serves to unambiguously identify individuals or subjects other than natural persons residing in Italy. Designed by and for the Italian tax Agency, it is now used for several other purposes, e.g. uniquely identifying individuals in the health system, or subjects who act as parties in public or private contracts. The code is issued by the Italian tax Agency</t>
+  </si>
+  <si>
+    <t>PARTITA IVA</t>
+  </si>
+  <si>
+    <t>The code is 11 numeric digits
+First 7 digits is a progressive number
+The following 3 digits means the province of residence
+The last digit is a check number, calculated using Luhn's Algorithm</t>
+  </si>
+  <si>
+    <t>Character Repertoire: 0 to 9</t>
+  </si>
+  <si>
+    <t>VAT registration number is an identifier used for value added tax purposes</t>
   </si>
 </sst>
 </file>
@@ -1912,6 +1962,60 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1333500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01CC2018-35F1-4C40-A115-D838395D8EEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9734550" cy="9525000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2260,13 +2364,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMM85"/>
+  <dimension ref="A1:AMM87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4351,84 +4455,2119 @@
       <c r="AML29" s="12"/>
       <c r="AMM29" s="12"/>
     </row>
-    <row r="30" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>16</v>
+    <row r="30" spans="1:1027" ht="285" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>479</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>475</v>
       </c>
       <c r="G30" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
+      <c r="H30" s="12"/>
       <c r="I30" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>16</v>
+        <v>483</v>
+      </c>
+      <c r="K30" s="15"/>
+      <c r="L30" s="13" t="s">
+        <v>484</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="12"/>
+      <c r="AA30" s="12"/>
+      <c r="AB30" s="12"/>
+      <c r="AC30" s="12"/>
+      <c r="AD30" s="12"/>
+      <c r="AE30" s="12"/>
+      <c r="AF30" s="12"/>
+      <c r="AG30" s="12"/>
+      <c r="AH30" s="12"/>
+      <c r="AI30" s="12"/>
+      <c r="AJ30" s="12"/>
+      <c r="AK30" s="12"/>
+      <c r="AL30" s="12"/>
+      <c r="AM30" s="12"/>
+      <c r="AN30" s="12"/>
+      <c r="AO30" s="12"/>
+      <c r="AP30" s="12"/>
+      <c r="AQ30" s="12"/>
+      <c r="AR30" s="12"/>
+      <c r="AS30" s="12"/>
+      <c r="AT30" s="12"/>
+      <c r="AU30" s="12"/>
+      <c r="AV30" s="12"/>
+      <c r="AW30" s="12"/>
+      <c r="AX30" s="12"/>
+      <c r="AY30" s="12"/>
+      <c r="AZ30" s="12"/>
+      <c r="BA30" s="12"/>
+      <c r="BB30" s="12"/>
+      <c r="BC30" s="12"/>
+      <c r="BD30" s="12"/>
+      <c r="BE30" s="12"/>
+      <c r="BF30" s="12"/>
+      <c r="BG30" s="12"/>
+      <c r="BH30" s="12"/>
+      <c r="BI30" s="12"/>
+      <c r="BJ30" s="12"/>
+      <c r="BK30" s="12"/>
+      <c r="BL30" s="12"/>
+      <c r="BM30" s="12"/>
+      <c r="BN30" s="12"/>
+      <c r="BO30" s="12"/>
+      <c r="BP30" s="12"/>
+      <c r="BQ30" s="12"/>
+      <c r="BR30" s="12"/>
+      <c r="BS30" s="12"/>
+      <c r="BT30" s="12"/>
+      <c r="BU30" s="12"/>
+      <c r="BV30" s="12"/>
+      <c r="BW30" s="12"/>
+      <c r="BX30" s="12"/>
+      <c r="BY30" s="12"/>
+      <c r="BZ30" s="12"/>
+      <c r="CA30" s="12"/>
+      <c r="CB30" s="12"/>
+      <c r="CC30" s="12"/>
+      <c r="CD30" s="12"/>
+      <c r="CE30" s="12"/>
+      <c r="CF30" s="12"/>
+      <c r="CG30" s="12"/>
+      <c r="CH30" s="12"/>
+      <c r="CI30" s="12"/>
+      <c r="CJ30" s="12"/>
+      <c r="CK30" s="12"/>
+      <c r="CL30" s="12"/>
+      <c r="CM30" s="12"/>
+      <c r="CN30" s="12"/>
+      <c r="CO30" s="12"/>
+      <c r="CP30" s="12"/>
+      <c r="CQ30" s="12"/>
+      <c r="CR30" s="12"/>
+      <c r="CS30" s="12"/>
+      <c r="CT30" s="12"/>
+      <c r="CU30" s="12"/>
+      <c r="CV30" s="12"/>
+      <c r="CW30" s="12"/>
+      <c r="CX30" s="12"/>
+      <c r="CY30" s="12"/>
+      <c r="CZ30" s="12"/>
+      <c r="DA30" s="12"/>
+      <c r="DB30" s="12"/>
+      <c r="DC30" s="12"/>
+      <c r="DD30" s="12"/>
+      <c r="DE30" s="12"/>
+      <c r="DF30" s="12"/>
+      <c r="DG30" s="12"/>
+      <c r="DH30" s="12"/>
+      <c r="DI30" s="12"/>
+      <c r="DJ30" s="12"/>
+      <c r="DK30" s="12"/>
+      <c r="DL30" s="12"/>
+      <c r="DM30" s="12"/>
+      <c r="DN30" s="12"/>
+      <c r="DO30" s="12"/>
+      <c r="DP30" s="12"/>
+      <c r="DQ30" s="12"/>
+      <c r="DR30" s="12"/>
+      <c r="DS30" s="12"/>
+      <c r="DT30" s="12"/>
+      <c r="DU30" s="12"/>
+      <c r="DV30" s="12"/>
+      <c r="DW30" s="12"/>
+      <c r="DX30" s="12"/>
+      <c r="DY30" s="12"/>
+      <c r="DZ30" s="12"/>
+      <c r="EA30" s="12"/>
+      <c r="EB30" s="12"/>
+      <c r="EC30" s="12"/>
+      <c r="ED30" s="12"/>
+      <c r="EE30" s="12"/>
+      <c r="EF30" s="12"/>
+      <c r="EG30" s="12"/>
+      <c r="EH30" s="12"/>
+      <c r="EI30" s="12"/>
+      <c r="EJ30" s="12"/>
+      <c r="EK30" s="12"/>
+      <c r="EL30" s="12"/>
+      <c r="EM30" s="12"/>
+      <c r="EN30" s="12"/>
+      <c r="EO30" s="12"/>
+      <c r="EP30" s="12"/>
+      <c r="EQ30" s="12"/>
+      <c r="ER30" s="12"/>
+      <c r="ES30" s="12"/>
+      <c r="ET30" s="12"/>
+      <c r="EU30" s="12"/>
+      <c r="EV30" s="12"/>
+      <c r="EW30" s="12"/>
+      <c r="EX30" s="12"/>
+      <c r="EY30" s="12"/>
+      <c r="EZ30" s="12"/>
+      <c r="FA30" s="12"/>
+      <c r="FB30" s="12"/>
+      <c r="FC30" s="12"/>
+      <c r="FD30" s="12"/>
+      <c r="FE30" s="12"/>
+      <c r="FF30" s="12"/>
+      <c r="FG30" s="12"/>
+      <c r="FH30" s="12"/>
+      <c r="FI30" s="12"/>
+      <c r="FJ30" s="12"/>
+      <c r="FK30" s="12"/>
+      <c r="FL30" s="12"/>
+      <c r="FM30" s="12"/>
+      <c r="FN30" s="12"/>
+      <c r="FO30" s="12"/>
+      <c r="FP30" s="12"/>
+      <c r="FQ30" s="12"/>
+      <c r="FR30" s="12"/>
+      <c r="FS30" s="12"/>
+      <c r="FT30" s="12"/>
+      <c r="FU30" s="12"/>
+      <c r="FV30" s="12"/>
+      <c r="FW30" s="12"/>
+      <c r="FX30" s="12"/>
+      <c r="FY30" s="12"/>
+      <c r="FZ30" s="12"/>
+      <c r="GA30" s="12"/>
+      <c r="GB30" s="12"/>
+      <c r="GC30" s="12"/>
+      <c r="GD30" s="12"/>
+      <c r="GE30" s="12"/>
+      <c r="GF30" s="12"/>
+      <c r="GG30" s="12"/>
+      <c r="GH30" s="12"/>
+      <c r="GI30" s="12"/>
+      <c r="GJ30" s="12"/>
+      <c r="GK30" s="12"/>
+      <c r="GL30" s="12"/>
+      <c r="GM30" s="12"/>
+      <c r="GN30" s="12"/>
+      <c r="GO30" s="12"/>
+      <c r="GP30" s="12"/>
+      <c r="GQ30" s="12"/>
+      <c r="GR30" s="12"/>
+      <c r="GS30" s="12"/>
+      <c r="GT30" s="12"/>
+      <c r="GU30" s="12"/>
+      <c r="GV30" s="12"/>
+      <c r="GW30" s="12"/>
+      <c r="GX30" s="12"/>
+      <c r="GY30" s="12"/>
+      <c r="GZ30" s="12"/>
+      <c r="HA30" s="12"/>
+      <c r="HB30" s="12"/>
+      <c r="HC30" s="12"/>
+      <c r="HD30" s="12"/>
+      <c r="HE30" s="12"/>
+      <c r="HF30" s="12"/>
+      <c r="HG30" s="12"/>
+      <c r="HH30" s="12"/>
+      <c r="HI30" s="12"/>
+      <c r="HJ30" s="12"/>
+      <c r="HK30" s="12"/>
+      <c r="HL30" s="12"/>
+      <c r="HM30" s="12"/>
+      <c r="HN30" s="12"/>
+      <c r="HO30" s="12"/>
+      <c r="HP30" s="12"/>
+      <c r="HQ30" s="12"/>
+      <c r="HR30" s="12"/>
+      <c r="HS30" s="12"/>
+      <c r="HT30" s="12"/>
+      <c r="HU30" s="12"/>
+      <c r="HV30" s="12"/>
+      <c r="HW30" s="12"/>
+      <c r="HX30" s="12"/>
+      <c r="HY30" s="12"/>
+      <c r="HZ30" s="12"/>
+      <c r="IA30" s="12"/>
+      <c r="IB30" s="12"/>
+      <c r="IC30" s="12"/>
+      <c r="ID30" s="12"/>
+      <c r="IE30" s="12"/>
+      <c r="IF30" s="12"/>
+      <c r="IG30" s="12"/>
+      <c r="IH30" s="12"/>
+      <c r="II30" s="12"/>
+      <c r="IJ30" s="12"/>
+      <c r="IK30" s="12"/>
+      <c r="IL30" s="12"/>
+      <c r="IM30" s="12"/>
+      <c r="IN30" s="12"/>
+      <c r="IO30" s="12"/>
+      <c r="IP30" s="12"/>
+      <c r="IQ30" s="12"/>
+      <c r="IR30" s="12"/>
+      <c r="IS30" s="12"/>
+      <c r="IT30" s="12"/>
+      <c r="IU30" s="12"/>
+      <c r="IV30" s="12"/>
+      <c r="IW30" s="12"/>
+      <c r="IX30" s="12"/>
+      <c r="IY30" s="12"/>
+      <c r="IZ30" s="12"/>
+      <c r="JA30" s="12"/>
+      <c r="JB30" s="12"/>
+      <c r="JC30" s="12"/>
+      <c r="JD30" s="12"/>
+      <c r="JE30" s="12"/>
+      <c r="JF30" s="12"/>
+      <c r="JG30" s="12"/>
+      <c r="JH30" s="12"/>
+      <c r="JI30" s="12"/>
+      <c r="JJ30" s="12"/>
+      <c r="JK30" s="12"/>
+      <c r="JL30" s="12"/>
+      <c r="JM30" s="12"/>
+      <c r="JN30" s="12"/>
+      <c r="JO30" s="12"/>
+      <c r="JP30" s="12"/>
+      <c r="JQ30" s="12"/>
+      <c r="JR30" s="12"/>
+      <c r="JS30" s="12"/>
+      <c r="JT30" s="12"/>
+      <c r="JU30" s="12"/>
+      <c r="JV30" s="12"/>
+      <c r="JW30" s="12"/>
+      <c r="JX30" s="12"/>
+      <c r="JY30" s="12"/>
+      <c r="JZ30" s="12"/>
+      <c r="KA30" s="12"/>
+      <c r="KB30" s="12"/>
+      <c r="KC30" s="12"/>
+      <c r="KD30" s="12"/>
+      <c r="KE30" s="12"/>
+      <c r="KF30" s="12"/>
+      <c r="KG30" s="12"/>
+      <c r="KH30" s="12"/>
+      <c r="KI30" s="12"/>
+      <c r="KJ30" s="12"/>
+      <c r="KK30" s="12"/>
+      <c r="KL30" s="12"/>
+      <c r="KM30" s="12"/>
+      <c r="KN30" s="12"/>
+      <c r="KO30" s="12"/>
+      <c r="KP30" s="12"/>
+      <c r="KQ30" s="12"/>
+      <c r="KR30" s="12"/>
+      <c r="KS30" s="12"/>
+      <c r="KT30" s="12"/>
+      <c r="KU30" s="12"/>
+      <c r="KV30" s="12"/>
+      <c r="KW30" s="12"/>
+      <c r="KX30" s="12"/>
+      <c r="KY30" s="12"/>
+      <c r="KZ30" s="12"/>
+      <c r="LA30" s="12"/>
+      <c r="LB30" s="12"/>
+      <c r="LC30" s="12"/>
+      <c r="LD30" s="12"/>
+      <c r="LE30" s="12"/>
+      <c r="LF30" s="12"/>
+      <c r="LG30" s="12"/>
+      <c r="LH30" s="12"/>
+      <c r="LI30" s="12"/>
+      <c r="LJ30" s="12"/>
+      <c r="LK30" s="12"/>
+      <c r="LL30" s="12"/>
+      <c r="LM30" s="12"/>
+      <c r="LN30" s="12"/>
+      <c r="LO30" s="12"/>
+      <c r="LP30" s="12"/>
+      <c r="LQ30" s="12"/>
+      <c r="LR30" s="12"/>
+      <c r="LS30" s="12"/>
+      <c r="LT30" s="12"/>
+      <c r="LU30" s="12"/>
+      <c r="LV30" s="12"/>
+      <c r="LW30" s="12"/>
+      <c r="LX30" s="12"/>
+      <c r="LY30" s="12"/>
+      <c r="LZ30" s="12"/>
+      <c r="MA30" s="12"/>
+      <c r="MB30" s="12"/>
+      <c r="MC30" s="12"/>
+      <c r="MD30" s="12"/>
+      <c r="ME30" s="12"/>
+      <c r="MF30" s="12"/>
+      <c r="MG30" s="12"/>
+      <c r="MH30" s="12"/>
+      <c r="MI30" s="12"/>
+      <c r="MJ30" s="12"/>
+      <c r="MK30" s="12"/>
+      <c r="ML30" s="12"/>
+      <c r="MM30" s="12"/>
+      <c r="MN30" s="12"/>
+      <c r="MO30" s="12"/>
+      <c r="MP30" s="12"/>
+      <c r="MQ30" s="12"/>
+      <c r="MR30" s="12"/>
+      <c r="MS30" s="12"/>
+      <c r="MT30" s="12"/>
+      <c r="MU30" s="12"/>
+      <c r="MV30" s="12"/>
+      <c r="MW30" s="12"/>
+      <c r="MX30" s="12"/>
+      <c r="MY30" s="12"/>
+      <c r="MZ30" s="12"/>
+      <c r="NA30" s="12"/>
+      <c r="NB30" s="12"/>
+      <c r="NC30" s="12"/>
+      <c r="ND30" s="12"/>
+      <c r="NE30" s="12"/>
+      <c r="NF30" s="12"/>
+      <c r="NG30" s="12"/>
+      <c r="NH30" s="12"/>
+      <c r="NI30" s="12"/>
+      <c r="NJ30" s="12"/>
+      <c r="NK30" s="12"/>
+      <c r="NL30" s="12"/>
+      <c r="NM30" s="12"/>
+      <c r="NN30" s="12"/>
+      <c r="NO30" s="12"/>
+      <c r="NP30" s="12"/>
+      <c r="NQ30" s="12"/>
+      <c r="NR30" s="12"/>
+      <c r="NS30" s="12"/>
+      <c r="NT30" s="12"/>
+      <c r="NU30" s="12"/>
+      <c r="NV30" s="12"/>
+      <c r="NW30" s="12"/>
+      <c r="NX30" s="12"/>
+      <c r="NY30" s="12"/>
+      <c r="NZ30" s="12"/>
+      <c r="OA30" s="12"/>
+      <c r="OB30" s="12"/>
+      <c r="OC30" s="12"/>
+      <c r="OD30" s="12"/>
+      <c r="OE30" s="12"/>
+      <c r="OF30" s="12"/>
+      <c r="OG30" s="12"/>
+      <c r="OH30" s="12"/>
+      <c r="OI30" s="12"/>
+      <c r="OJ30" s="12"/>
+      <c r="OK30" s="12"/>
+      <c r="OL30" s="12"/>
+      <c r="OM30" s="12"/>
+      <c r="ON30" s="12"/>
+      <c r="OO30" s="12"/>
+      <c r="OP30" s="12"/>
+      <c r="OQ30" s="12"/>
+      <c r="OR30" s="12"/>
+      <c r="OS30" s="12"/>
+      <c r="OT30" s="12"/>
+      <c r="OU30" s="12"/>
+      <c r="OV30" s="12"/>
+      <c r="OW30" s="12"/>
+      <c r="OX30" s="12"/>
+      <c r="OY30" s="12"/>
+      <c r="OZ30" s="12"/>
+      <c r="PA30" s="12"/>
+      <c r="PB30" s="12"/>
+      <c r="PC30" s="12"/>
+      <c r="PD30" s="12"/>
+      <c r="PE30" s="12"/>
+      <c r="PF30" s="12"/>
+      <c r="PG30" s="12"/>
+      <c r="PH30" s="12"/>
+      <c r="PI30" s="12"/>
+      <c r="PJ30" s="12"/>
+      <c r="PK30" s="12"/>
+      <c r="PL30" s="12"/>
+      <c r="PM30" s="12"/>
+      <c r="PN30" s="12"/>
+      <c r="PO30" s="12"/>
+      <c r="PP30" s="12"/>
+      <c r="PQ30" s="12"/>
+      <c r="PR30" s="12"/>
+      <c r="PS30" s="12"/>
+      <c r="PT30" s="12"/>
+      <c r="PU30" s="12"/>
+      <c r="PV30" s="12"/>
+      <c r="PW30" s="12"/>
+      <c r="PX30" s="12"/>
+      <c r="PY30" s="12"/>
+      <c r="PZ30" s="12"/>
+      <c r="QA30" s="12"/>
+      <c r="QB30" s="12"/>
+      <c r="QC30" s="12"/>
+      <c r="QD30" s="12"/>
+      <c r="QE30" s="12"/>
+      <c r="QF30" s="12"/>
+      <c r="QG30" s="12"/>
+      <c r="QH30" s="12"/>
+      <c r="QI30" s="12"/>
+      <c r="QJ30" s="12"/>
+      <c r="QK30" s="12"/>
+      <c r="QL30" s="12"/>
+      <c r="QM30" s="12"/>
+      <c r="QN30" s="12"/>
+      <c r="QO30" s="12"/>
+      <c r="QP30" s="12"/>
+      <c r="QQ30" s="12"/>
+      <c r="QR30" s="12"/>
+      <c r="QS30" s="12"/>
+      <c r="QT30" s="12"/>
+      <c r="QU30" s="12"/>
+      <c r="QV30" s="12"/>
+      <c r="QW30" s="12"/>
+      <c r="QX30" s="12"/>
+      <c r="QY30" s="12"/>
+      <c r="QZ30" s="12"/>
+      <c r="RA30" s="12"/>
+      <c r="RB30" s="12"/>
+      <c r="RC30" s="12"/>
+      <c r="RD30" s="12"/>
+      <c r="RE30" s="12"/>
+      <c r="RF30" s="12"/>
+      <c r="RG30" s="12"/>
+      <c r="RH30" s="12"/>
+      <c r="RI30" s="12"/>
+      <c r="RJ30" s="12"/>
+      <c r="RK30" s="12"/>
+      <c r="RL30" s="12"/>
+      <c r="RM30" s="12"/>
+      <c r="RN30" s="12"/>
+      <c r="RO30" s="12"/>
+      <c r="RP30" s="12"/>
+      <c r="RQ30" s="12"/>
+      <c r="RR30" s="12"/>
+      <c r="RS30" s="12"/>
+      <c r="RT30" s="12"/>
+      <c r="RU30" s="12"/>
+      <c r="RV30" s="12"/>
+      <c r="RW30" s="12"/>
+      <c r="RX30" s="12"/>
+      <c r="RY30" s="12"/>
+      <c r="RZ30" s="12"/>
+      <c r="SA30" s="12"/>
+      <c r="SB30" s="12"/>
+      <c r="SC30" s="12"/>
+      <c r="SD30" s="12"/>
+      <c r="SE30" s="12"/>
+      <c r="SF30" s="12"/>
+      <c r="SG30" s="12"/>
+      <c r="SH30" s="12"/>
+      <c r="SI30" s="12"/>
+      <c r="SJ30" s="12"/>
+      <c r="SK30" s="12"/>
+      <c r="SL30" s="12"/>
+      <c r="SM30" s="12"/>
+      <c r="SN30" s="12"/>
+      <c r="SO30" s="12"/>
+      <c r="SP30" s="12"/>
+      <c r="SQ30" s="12"/>
+      <c r="SR30" s="12"/>
+      <c r="SS30" s="12"/>
+      <c r="ST30" s="12"/>
+      <c r="SU30" s="12"/>
+      <c r="SV30" s="12"/>
+      <c r="SW30" s="12"/>
+      <c r="SX30" s="12"/>
+      <c r="SY30" s="12"/>
+      <c r="SZ30" s="12"/>
+      <c r="TA30" s="12"/>
+      <c r="TB30" s="12"/>
+      <c r="TC30" s="12"/>
+      <c r="TD30" s="12"/>
+      <c r="TE30" s="12"/>
+      <c r="TF30" s="12"/>
+      <c r="TG30" s="12"/>
+      <c r="TH30" s="12"/>
+      <c r="TI30" s="12"/>
+      <c r="TJ30" s="12"/>
+      <c r="TK30" s="12"/>
+      <c r="TL30" s="12"/>
+      <c r="TM30" s="12"/>
+      <c r="TN30" s="12"/>
+      <c r="TO30" s="12"/>
+      <c r="TP30" s="12"/>
+      <c r="TQ30" s="12"/>
+      <c r="TR30" s="12"/>
+      <c r="TS30" s="12"/>
+      <c r="TT30" s="12"/>
+      <c r="TU30" s="12"/>
+      <c r="TV30" s="12"/>
+      <c r="TW30" s="12"/>
+      <c r="TX30" s="12"/>
+      <c r="TY30" s="12"/>
+      <c r="TZ30" s="12"/>
+      <c r="UA30" s="12"/>
+      <c r="UB30" s="12"/>
+      <c r="UC30" s="12"/>
+      <c r="UD30" s="12"/>
+      <c r="UE30" s="12"/>
+      <c r="UF30" s="12"/>
+      <c r="UG30" s="12"/>
+      <c r="UH30" s="12"/>
+      <c r="UI30" s="12"/>
+      <c r="UJ30" s="12"/>
+      <c r="UK30" s="12"/>
+      <c r="UL30" s="12"/>
+      <c r="UM30" s="12"/>
+      <c r="UN30" s="12"/>
+      <c r="UO30" s="12"/>
+      <c r="UP30" s="12"/>
+      <c r="UQ30" s="12"/>
+      <c r="UR30" s="12"/>
+      <c r="US30" s="12"/>
+      <c r="UT30" s="12"/>
+      <c r="UU30" s="12"/>
+      <c r="UV30" s="12"/>
+      <c r="UW30" s="12"/>
+      <c r="UX30" s="12"/>
+      <c r="UY30" s="12"/>
+      <c r="UZ30" s="12"/>
+      <c r="VA30" s="12"/>
+      <c r="VB30" s="12"/>
+      <c r="VC30" s="12"/>
+      <c r="VD30" s="12"/>
+      <c r="VE30" s="12"/>
+      <c r="VF30" s="12"/>
+      <c r="VG30" s="12"/>
+      <c r="VH30" s="12"/>
+      <c r="VI30" s="12"/>
+      <c r="VJ30" s="12"/>
+      <c r="VK30" s="12"/>
+      <c r="VL30" s="12"/>
+      <c r="VM30" s="12"/>
+      <c r="VN30" s="12"/>
+      <c r="VO30" s="12"/>
+      <c r="VP30" s="12"/>
+      <c r="VQ30" s="12"/>
+      <c r="VR30" s="12"/>
+      <c r="VS30" s="12"/>
+      <c r="VT30" s="12"/>
+      <c r="VU30" s="12"/>
+      <c r="VV30" s="12"/>
+      <c r="VW30" s="12"/>
+      <c r="VX30" s="12"/>
+      <c r="VY30" s="12"/>
+      <c r="VZ30" s="12"/>
+      <c r="WA30" s="12"/>
+      <c r="WB30" s="12"/>
+      <c r="WC30" s="12"/>
+      <c r="WD30" s="12"/>
+      <c r="WE30" s="12"/>
+      <c r="WF30" s="12"/>
+      <c r="WG30" s="12"/>
+      <c r="WH30" s="12"/>
+      <c r="WI30" s="12"/>
+      <c r="WJ30" s="12"/>
+      <c r="WK30" s="12"/>
+      <c r="WL30" s="12"/>
+      <c r="WM30" s="12"/>
+      <c r="WN30" s="12"/>
+      <c r="WO30" s="12"/>
+      <c r="WP30" s="12"/>
+      <c r="WQ30" s="12"/>
+      <c r="WR30" s="12"/>
+      <c r="WS30" s="12"/>
+      <c r="WT30" s="12"/>
+      <c r="WU30" s="12"/>
+      <c r="WV30" s="12"/>
+      <c r="WW30" s="12"/>
+      <c r="WX30" s="12"/>
+      <c r="WY30" s="12"/>
+      <c r="WZ30" s="12"/>
+      <c r="XA30" s="12"/>
+      <c r="XB30" s="12"/>
+      <c r="XC30" s="12"/>
+      <c r="XD30" s="12"/>
+      <c r="XE30" s="12"/>
+      <c r="XF30" s="12"/>
+      <c r="XG30" s="12"/>
+      <c r="XH30" s="12"/>
+      <c r="XI30" s="12"/>
+      <c r="XJ30" s="12"/>
+      <c r="XK30" s="12"/>
+      <c r="XL30" s="12"/>
+      <c r="XM30" s="12"/>
+      <c r="XN30" s="12"/>
+      <c r="XO30" s="12"/>
+      <c r="XP30" s="12"/>
+      <c r="XQ30" s="12"/>
+      <c r="XR30" s="12"/>
+      <c r="XS30" s="12"/>
+      <c r="XT30" s="12"/>
+      <c r="XU30" s="12"/>
+      <c r="XV30" s="12"/>
+      <c r="XW30" s="12"/>
+      <c r="XX30" s="12"/>
+      <c r="XY30" s="12"/>
+      <c r="XZ30" s="12"/>
+      <c r="YA30" s="12"/>
+      <c r="YB30" s="12"/>
+      <c r="YC30" s="12"/>
+      <c r="YD30" s="12"/>
+      <c r="YE30" s="12"/>
+      <c r="YF30" s="12"/>
+      <c r="YG30" s="12"/>
+      <c r="YH30" s="12"/>
+      <c r="YI30" s="12"/>
+      <c r="YJ30" s="12"/>
+      <c r="YK30" s="12"/>
+      <c r="YL30" s="12"/>
+      <c r="YM30" s="12"/>
+      <c r="YN30" s="12"/>
+      <c r="YO30" s="12"/>
+      <c r="YP30" s="12"/>
+      <c r="YQ30" s="12"/>
+      <c r="YR30" s="12"/>
+      <c r="YS30" s="12"/>
+      <c r="YT30" s="12"/>
+      <c r="YU30" s="12"/>
+      <c r="YV30" s="12"/>
+      <c r="YW30" s="12"/>
+      <c r="YX30" s="12"/>
+      <c r="YY30" s="12"/>
+      <c r="YZ30" s="12"/>
+      <c r="ZA30" s="12"/>
+      <c r="ZB30" s="12"/>
+      <c r="ZC30" s="12"/>
+      <c r="ZD30" s="12"/>
+      <c r="ZE30" s="12"/>
+      <c r="ZF30" s="12"/>
+      <c r="ZG30" s="12"/>
+      <c r="ZH30" s="12"/>
+      <c r="ZI30" s="12"/>
+      <c r="ZJ30" s="12"/>
+      <c r="ZK30" s="12"/>
+      <c r="ZL30" s="12"/>
+      <c r="ZM30" s="12"/>
+      <c r="ZN30" s="12"/>
+      <c r="ZO30" s="12"/>
+      <c r="ZP30" s="12"/>
+      <c r="ZQ30" s="12"/>
+      <c r="ZR30" s="12"/>
+      <c r="ZS30" s="12"/>
+      <c r="ZT30" s="12"/>
+      <c r="ZU30" s="12"/>
+      <c r="ZV30" s="12"/>
+      <c r="ZW30" s="12"/>
+      <c r="ZX30" s="12"/>
+      <c r="ZY30" s="12"/>
+      <c r="ZZ30" s="12"/>
+      <c r="AAA30" s="12"/>
+      <c r="AAB30" s="12"/>
+      <c r="AAC30" s="12"/>
+      <c r="AAD30" s="12"/>
+      <c r="AAE30" s="12"/>
+      <c r="AAF30" s="12"/>
+      <c r="AAG30" s="12"/>
+      <c r="AAH30" s="12"/>
+      <c r="AAI30" s="12"/>
+      <c r="AAJ30" s="12"/>
+      <c r="AAK30" s="12"/>
+      <c r="AAL30" s="12"/>
+      <c r="AAM30" s="12"/>
+      <c r="AAN30" s="12"/>
+      <c r="AAO30" s="12"/>
+      <c r="AAP30" s="12"/>
+      <c r="AAQ30" s="12"/>
+      <c r="AAR30" s="12"/>
+      <c r="AAS30" s="12"/>
+      <c r="AAT30" s="12"/>
+      <c r="AAU30" s="12"/>
+      <c r="AAV30" s="12"/>
+      <c r="AAW30" s="12"/>
+      <c r="AAX30" s="12"/>
+      <c r="AAY30" s="12"/>
+      <c r="AAZ30" s="12"/>
+      <c r="ABA30" s="12"/>
+      <c r="ABB30" s="12"/>
+      <c r="ABC30" s="12"/>
+      <c r="ABD30" s="12"/>
+      <c r="ABE30" s="12"/>
+      <c r="ABF30" s="12"/>
+      <c r="ABG30" s="12"/>
+      <c r="ABH30" s="12"/>
+      <c r="ABI30" s="12"/>
+      <c r="ABJ30" s="12"/>
+      <c r="ABK30" s="12"/>
+      <c r="ABL30" s="12"/>
+      <c r="ABM30" s="12"/>
+      <c r="ABN30" s="12"/>
+      <c r="ABO30" s="12"/>
+      <c r="ABP30" s="12"/>
+      <c r="ABQ30" s="12"/>
+      <c r="ABR30" s="12"/>
+      <c r="ABS30" s="12"/>
+      <c r="ABT30" s="12"/>
+      <c r="ABU30" s="12"/>
+      <c r="ABV30" s="12"/>
+      <c r="ABW30" s="12"/>
+      <c r="ABX30" s="12"/>
+      <c r="ABY30" s="12"/>
+      <c r="ABZ30" s="12"/>
+      <c r="ACA30" s="12"/>
+      <c r="ACB30" s="12"/>
+      <c r="ACC30" s="12"/>
+      <c r="ACD30" s="12"/>
+      <c r="ACE30" s="12"/>
+      <c r="ACF30" s="12"/>
+      <c r="ACG30" s="12"/>
+      <c r="ACH30" s="12"/>
+      <c r="ACI30" s="12"/>
+      <c r="ACJ30" s="12"/>
+      <c r="ACK30" s="12"/>
+      <c r="ACL30" s="12"/>
+      <c r="ACM30" s="12"/>
+      <c r="ACN30" s="12"/>
+      <c r="ACO30" s="12"/>
+      <c r="ACP30" s="12"/>
+      <c r="ACQ30" s="12"/>
+      <c r="ACR30" s="12"/>
+      <c r="ACS30" s="12"/>
+      <c r="ACT30" s="12"/>
+      <c r="ACU30" s="12"/>
+      <c r="ACV30" s="12"/>
+      <c r="ACW30" s="12"/>
+      <c r="ACX30" s="12"/>
+      <c r="ACY30" s="12"/>
+      <c r="ACZ30" s="12"/>
+      <c r="ADA30" s="12"/>
+      <c r="ADB30" s="12"/>
+      <c r="ADC30" s="12"/>
+      <c r="ADD30" s="12"/>
+      <c r="ADE30" s="12"/>
+      <c r="ADF30" s="12"/>
+      <c r="ADG30" s="12"/>
+      <c r="ADH30" s="12"/>
+      <c r="ADI30" s="12"/>
+      <c r="ADJ30" s="12"/>
+      <c r="ADK30" s="12"/>
+      <c r="ADL30" s="12"/>
+      <c r="ADM30" s="12"/>
+      <c r="ADN30" s="12"/>
+      <c r="ADO30" s="12"/>
+      <c r="ADP30" s="12"/>
+      <c r="ADQ30" s="12"/>
+      <c r="ADR30" s="12"/>
+      <c r="ADS30" s="12"/>
+      <c r="ADT30" s="12"/>
+      <c r="ADU30" s="12"/>
+      <c r="ADV30" s="12"/>
+      <c r="ADW30" s="12"/>
+      <c r="ADX30" s="12"/>
+      <c r="ADY30" s="12"/>
+      <c r="ADZ30" s="12"/>
+      <c r="AEA30" s="12"/>
+      <c r="AEB30" s="12"/>
+      <c r="AEC30" s="12"/>
+      <c r="AED30" s="12"/>
+      <c r="AEE30" s="12"/>
+      <c r="AEF30" s="12"/>
+      <c r="AEG30" s="12"/>
+      <c r="AEH30" s="12"/>
+      <c r="AEI30" s="12"/>
+      <c r="AEJ30" s="12"/>
+      <c r="AEK30" s="12"/>
+      <c r="AEL30" s="12"/>
+      <c r="AEM30" s="12"/>
+      <c r="AEN30" s="12"/>
+      <c r="AEO30" s="12"/>
+      <c r="AEP30" s="12"/>
+      <c r="AEQ30" s="12"/>
+      <c r="AER30" s="12"/>
+      <c r="AES30" s="12"/>
+      <c r="AET30" s="12"/>
+      <c r="AEU30" s="12"/>
+      <c r="AEV30" s="12"/>
+      <c r="AEW30" s="12"/>
+      <c r="AEX30" s="12"/>
+      <c r="AEY30" s="12"/>
+      <c r="AEZ30" s="12"/>
+      <c r="AFA30" s="12"/>
+      <c r="AFB30" s="12"/>
+      <c r="AFC30" s="12"/>
+      <c r="AFD30" s="12"/>
+      <c r="AFE30" s="12"/>
+      <c r="AFF30" s="12"/>
+      <c r="AFG30" s="12"/>
+      <c r="AFH30" s="12"/>
+      <c r="AFI30" s="12"/>
+      <c r="AFJ30" s="12"/>
+      <c r="AFK30" s="12"/>
+      <c r="AFL30" s="12"/>
+      <c r="AFM30" s="12"/>
+      <c r="AFN30" s="12"/>
+      <c r="AFO30" s="12"/>
+      <c r="AFP30" s="12"/>
+      <c r="AFQ30" s="12"/>
+      <c r="AFR30" s="12"/>
+      <c r="AFS30" s="12"/>
+      <c r="AFT30" s="12"/>
+      <c r="AFU30" s="12"/>
+      <c r="AFV30" s="12"/>
+      <c r="AFW30" s="12"/>
+      <c r="AFX30" s="12"/>
+      <c r="AFY30" s="12"/>
+      <c r="AFZ30" s="12"/>
+      <c r="AGA30" s="12"/>
+      <c r="AGB30" s="12"/>
+      <c r="AGC30" s="12"/>
+      <c r="AGD30" s="12"/>
+      <c r="AGE30" s="12"/>
+      <c r="AGF30" s="12"/>
+      <c r="AGG30" s="12"/>
+      <c r="AGH30" s="12"/>
+      <c r="AGI30" s="12"/>
+      <c r="AGJ30" s="12"/>
+      <c r="AGK30" s="12"/>
+      <c r="AGL30" s="12"/>
+      <c r="AGM30" s="12"/>
+      <c r="AGN30" s="12"/>
+      <c r="AGO30" s="12"/>
+      <c r="AGP30" s="12"/>
+      <c r="AGQ30" s="12"/>
+      <c r="AGR30" s="12"/>
+      <c r="AGS30" s="12"/>
+      <c r="AGT30" s="12"/>
+      <c r="AGU30" s="12"/>
+      <c r="AGV30" s="12"/>
+      <c r="AGW30" s="12"/>
+      <c r="AGX30" s="12"/>
+      <c r="AGY30" s="12"/>
+      <c r="AGZ30" s="12"/>
+      <c r="AHA30" s="12"/>
+      <c r="AHB30" s="12"/>
+      <c r="AHC30" s="12"/>
+      <c r="AHD30" s="12"/>
+      <c r="AHE30" s="12"/>
+      <c r="AHF30" s="12"/>
+      <c r="AHG30" s="12"/>
+      <c r="AHH30" s="12"/>
+      <c r="AHI30" s="12"/>
+      <c r="AHJ30" s="12"/>
+      <c r="AHK30" s="12"/>
+      <c r="AHL30" s="12"/>
+      <c r="AHM30" s="12"/>
+      <c r="AHN30" s="12"/>
+      <c r="AHO30" s="12"/>
+      <c r="AHP30" s="12"/>
+      <c r="AHQ30" s="12"/>
+      <c r="AHR30" s="12"/>
+      <c r="AHS30" s="12"/>
+      <c r="AHT30" s="12"/>
+      <c r="AHU30" s="12"/>
+      <c r="AHV30" s="12"/>
+      <c r="AHW30" s="12"/>
+      <c r="AHX30" s="12"/>
+      <c r="AHY30" s="12"/>
+      <c r="AHZ30" s="12"/>
+      <c r="AIA30" s="12"/>
+      <c r="AIB30" s="12"/>
+      <c r="AIC30" s="12"/>
+      <c r="AID30" s="12"/>
+      <c r="AIE30" s="12"/>
+      <c r="AIF30" s="12"/>
+      <c r="AIG30" s="12"/>
+      <c r="AIH30" s="12"/>
+      <c r="AII30" s="12"/>
+      <c r="AIJ30" s="12"/>
+      <c r="AIK30" s="12"/>
+      <c r="AIL30" s="12"/>
+      <c r="AIM30" s="12"/>
+      <c r="AIN30" s="12"/>
+      <c r="AIO30" s="12"/>
+      <c r="AIP30" s="12"/>
+      <c r="AIQ30" s="12"/>
+      <c r="AIR30" s="12"/>
+      <c r="AIS30" s="12"/>
+      <c r="AIT30" s="12"/>
+      <c r="AIU30" s="12"/>
+      <c r="AIV30" s="12"/>
+      <c r="AIW30" s="12"/>
+      <c r="AIX30" s="12"/>
+      <c r="AIY30" s="12"/>
+      <c r="AIZ30" s="12"/>
+      <c r="AJA30" s="12"/>
+      <c r="AJB30" s="12"/>
+      <c r="AJC30" s="12"/>
+      <c r="AJD30" s="12"/>
+      <c r="AJE30" s="12"/>
+      <c r="AJF30" s="12"/>
+      <c r="AJG30" s="12"/>
+      <c r="AJH30" s="12"/>
+      <c r="AJI30" s="12"/>
+      <c r="AJJ30" s="12"/>
+      <c r="AJK30" s="12"/>
+      <c r="AJL30" s="12"/>
+      <c r="AJM30" s="12"/>
+      <c r="AJN30" s="12"/>
+      <c r="AJO30" s="12"/>
+      <c r="AJP30" s="12"/>
+      <c r="AJQ30" s="12"/>
+      <c r="AJR30" s="12"/>
+      <c r="AJS30" s="12"/>
+      <c r="AJT30" s="12"/>
+      <c r="AJU30" s="12"/>
+      <c r="AJV30" s="12"/>
+      <c r="AJW30" s="12"/>
+      <c r="AJX30" s="12"/>
+      <c r="AJY30" s="12"/>
+      <c r="AJZ30" s="12"/>
+      <c r="AKA30" s="12"/>
+      <c r="AKB30" s="12"/>
+      <c r="AKC30" s="12"/>
+      <c r="AKD30" s="12"/>
+      <c r="AKE30" s="12"/>
+      <c r="AKF30" s="12"/>
+      <c r="AKG30" s="12"/>
+      <c r="AKH30" s="12"/>
+      <c r="AKI30" s="12"/>
+      <c r="AKJ30" s="12"/>
+      <c r="AKK30" s="12"/>
+      <c r="AKL30" s="12"/>
+      <c r="AKM30" s="12"/>
+      <c r="AKN30" s="12"/>
+      <c r="AKO30" s="12"/>
+      <c r="AKP30" s="12"/>
+      <c r="AKQ30" s="12"/>
+      <c r="AKR30" s="12"/>
+      <c r="AKS30" s="12"/>
+      <c r="AKT30" s="12"/>
+      <c r="AKU30" s="12"/>
+      <c r="AKV30" s="12"/>
+      <c r="AKW30" s="12"/>
+      <c r="AKX30" s="12"/>
+      <c r="AKY30" s="12"/>
+      <c r="AKZ30" s="12"/>
+      <c r="ALA30" s="12"/>
+      <c r="ALB30" s="12"/>
+      <c r="ALC30" s="12"/>
+      <c r="ALD30" s="12"/>
+      <c r="ALE30" s="12"/>
+      <c r="ALF30" s="12"/>
+      <c r="ALG30" s="12"/>
+      <c r="ALH30" s="12"/>
+      <c r="ALI30" s="12"/>
+      <c r="ALJ30" s="12"/>
+      <c r="ALK30" s="12"/>
+      <c r="ALL30" s="12"/>
+      <c r="ALM30" s="12"/>
+      <c r="ALN30" s="12"/>
+      <c r="ALO30" s="12"/>
+      <c r="ALP30" s="12"/>
+      <c r="ALQ30" s="12"/>
+      <c r="ALR30" s="12"/>
+      <c r="ALS30" s="12"/>
+      <c r="ALT30" s="12"/>
+      <c r="ALU30" s="12"/>
+      <c r="ALV30" s="12"/>
+      <c r="ALW30" s="12"/>
+      <c r="ALX30" s="12"/>
+      <c r="ALY30" s="12"/>
+      <c r="ALZ30" s="12"/>
+      <c r="AMA30" s="12"/>
+      <c r="AMB30" s="12"/>
+      <c r="AMC30" s="12"/>
+      <c r="AMD30" s="12"/>
+      <c r="AME30" s="12"/>
+      <c r="AMF30" s="12"/>
+      <c r="AMG30" s="12"/>
+      <c r="AMH30" s="12"/>
+      <c r="AMI30" s="12"/>
+      <c r="AMJ30" s="12"/>
+      <c r="AMK30" s="12"/>
+      <c r="AML30" s="12"/>
+      <c r="AMM30" s="12"/>
+    </row>
+    <row r="31" spans="1:1027" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>480</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>486</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>482</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>475</v>
       </c>
       <c r="G31" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K31" s="2" t="s">
-        <v>405</v>
-      </c>
+      <c r="H31" s="12"/>
+      <c r="I31" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="K31" s="15"/>
       <c r="L31" s="13" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
+        <v>488</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>489</v>
+      </c>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12"/>
+      <c r="V31" s="12"/>
+      <c r="W31" s="12"/>
+      <c r="X31" s="12"/>
+      <c r="Y31" s="12"/>
+      <c r="Z31" s="12"/>
+      <c r="AA31" s="12"/>
+      <c r="AB31" s="12"/>
+      <c r="AC31" s="12"/>
+      <c r="AD31" s="12"/>
+      <c r="AE31" s="12"/>
+      <c r="AF31" s="12"/>
+      <c r="AG31" s="12"/>
+      <c r="AH31" s="12"/>
+      <c r="AI31" s="12"/>
+      <c r="AJ31" s="12"/>
+      <c r="AK31" s="12"/>
+      <c r="AL31" s="12"/>
+      <c r="AM31" s="12"/>
+      <c r="AN31" s="12"/>
+      <c r="AO31" s="12"/>
+      <c r="AP31" s="12"/>
+      <c r="AQ31" s="12"/>
+      <c r="AR31" s="12"/>
+      <c r="AS31" s="12"/>
+      <c r="AT31" s="12"/>
+      <c r="AU31" s="12"/>
+      <c r="AV31" s="12"/>
+      <c r="AW31" s="12"/>
+      <c r="AX31" s="12"/>
+      <c r="AY31" s="12"/>
+      <c r="AZ31" s="12"/>
+      <c r="BA31" s="12"/>
+      <c r="BB31" s="12"/>
+      <c r="BC31" s="12"/>
+      <c r="BD31" s="12"/>
+      <c r="BE31" s="12"/>
+      <c r="BF31" s="12"/>
+      <c r="BG31" s="12"/>
+      <c r="BH31" s="12"/>
+      <c r="BI31" s="12"/>
+      <c r="BJ31" s="12"/>
+      <c r="BK31" s="12"/>
+      <c r="BL31" s="12"/>
+      <c r="BM31" s="12"/>
+      <c r="BN31" s="12"/>
+      <c r="BO31" s="12"/>
+      <c r="BP31" s="12"/>
+      <c r="BQ31" s="12"/>
+      <c r="BR31" s="12"/>
+      <c r="BS31" s="12"/>
+      <c r="BT31" s="12"/>
+      <c r="BU31" s="12"/>
+      <c r="BV31" s="12"/>
+      <c r="BW31" s="12"/>
+      <c r="BX31" s="12"/>
+      <c r="BY31" s="12"/>
+      <c r="BZ31" s="12"/>
+      <c r="CA31" s="12"/>
+      <c r="CB31" s="12"/>
+      <c r="CC31" s="12"/>
+      <c r="CD31" s="12"/>
+      <c r="CE31" s="12"/>
+      <c r="CF31" s="12"/>
+      <c r="CG31" s="12"/>
+      <c r="CH31" s="12"/>
+      <c r="CI31" s="12"/>
+      <c r="CJ31" s="12"/>
+      <c r="CK31" s="12"/>
+      <c r="CL31" s="12"/>
+      <c r="CM31" s="12"/>
+      <c r="CN31" s="12"/>
+      <c r="CO31" s="12"/>
+      <c r="CP31" s="12"/>
+      <c r="CQ31" s="12"/>
+      <c r="CR31" s="12"/>
+      <c r="CS31" s="12"/>
+      <c r="CT31" s="12"/>
+      <c r="CU31" s="12"/>
+      <c r="CV31" s="12"/>
+      <c r="CW31" s="12"/>
+      <c r="CX31" s="12"/>
+      <c r="CY31" s="12"/>
+      <c r="CZ31" s="12"/>
+      <c r="DA31" s="12"/>
+      <c r="DB31" s="12"/>
+      <c r="DC31" s="12"/>
+      <c r="DD31" s="12"/>
+      <c r="DE31" s="12"/>
+      <c r="DF31" s="12"/>
+      <c r="DG31" s="12"/>
+      <c r="DH31" s="12"/>
+      <c r="DI31" s="12"/>
+      <c r="DJ31" s="12"/>
+      <c r="DK31" s="12"/>
+      <c r="DL31" s="12"/>
+      <c r="DM31" s="12"/>
+      <c r="DN31" s="12"/>
+      <c r="DO31" s="12"/>
+      <c r="DP31" s="12"/>
+      <c r="DQ31" s="12"/>
+      <c r="DR31" s="12"/>
+      <c r="DS31" s="12"/>
+      <c r="DT31" s="12"/>
+      <c r="DU31" s="12"/>
+      <c r="DV31" s="12"/>
+      <c r="DW31" s="12"/>
+      <c r="DX31" s="12"/>
+      <c r="DY31" s="12"/>
+      <c r="DZ31" s="12"/>
+      <c r="EA31" s="12"/>
+      <c r="EB31" s="12"/>
+      <c r="EC31" s="12"/>
+      <c r="ED31" s="12"/>
+      <c r="EE31" s="12"/>
+      <c r="EF31" s="12"/>
+      <c r="EG31" s="12"/>
+      <c r="EH31" s="12"/>
+      <c r="EI31" s="12"/>
+      <c r="EJ31" s="12"/>
+      <c r="EK31" s="12"/>
+      <c r="EL31" s="12"/>
+      <c r="EM31" s="12"/>
+      <c r="EN31" s="12"/>
+      <c r="EO31" s="12"/>
+      <c r="EP31" s="12"/>
+      <c r="EQ31" s="12"/>
+      <c r="ER31" s="12"/>
+      <c r="ES31" s="12"/>
+      <c r="ET31" s="12"/>
+      <c r="EU31" s="12"/>
+      <c r="EV31" s="12"/>
+      <c r="EW31" s="12"/>
+      <c r="EX31" s="12"/>
+      <c r="EY31" s="12"/>
+      <c r="EZ31" s="12"/>
+      <c r="FA31" s="12"/>
+      <c r="FB31" s="12"/>
+      <c r="FC31" s="12"/>
+      <c r="FD31" s="12"/>
+      <c r="FE31" s="12"/>
+      <c r="FF31" s="12"/>
+      <c r="FG31" s="12"/>
+      <c r="FH31" s="12"/>
+      <c r="FI31" s="12"/>
+      <c r="FJ31" s="12"/>
+      <c r="FK31" s="12"/>
+      <c r="FL31" s="12"/>
+      <c r="FM31" s="12"/>
+      <c r="FN31" s="12"/>
+      <c r="FO31" s="12"/>
+      <c r="FP31" s="12"/>
+      <c r="FQ31" s="12"/>
+      <c r="FR31" s="12"/>
+      <c r="FS31" s="12"/>
+      <c r="FT31" s="12"/>
+      <c r="FU31" s="12"/>
+      <c r="FV31" s="12"/>
+      <c r="FW31" s="12"/>
+      <c r="FX31" s="12"/>
+      <c r="FY31" s="12"/>
+      <c r="FZ31" s="12"/>
+      <c r="GA31" s="12"/>
+      <c r="GB31" s="12"/>
+      <c r="GC31" s="12"/>
+      <c r="GD31" s="12"/>
+      <c r="GE31" s="12"/>
+      <c r="GF31" s="12"/>
+      <c r="GG31" s="12"/>
+      <c r="GH31" s="12"/>
+      <c r="GI31" s="12"/>
+      <c r="GJ31" s="12"/>
+      <c r="GK31" s="12"/>
+      <c r="GL31" s="12"/>
+      <c r="GM31" s="12"/>
+      <c r="GN31" s="12"/>
+      <c r="GO31" s="12"/>
+      <c r="GP31" s="12"/>
+      <c r="GQ31" s="12"/>
+      <c r="GR31" s="12"/>
+      <c r="GS31" s="12"/>
+      <c r="GT31" s="12"/>
+      <c r="GU31" s="12"/>
+      <c r="GV31" s="12"/>
+      <c r="GW31" s="12"/>
+      <c r="GX31" s="12"/>
+      <c r="GY31" s="12"/>
+      <c r="GZ31" s="12"/>
+      <c r="HA31" s="12"/>
+      <c r="HB31" s="12"/>
+      <c r="HC31" s="12"/>
+      <c r="HD31" s="12"/>
+      <c r="HE31" s="12"/>
+      <c r="HF31" s="12"/>
+      <c r="HG31" s="12"/>
+      <c r="HH31" s="12"/>
+      <c r="HI31" s="12"/>
+      <c r="HJ31" s="12"/>
+      <c r="HK31" s="12"/>
+      <c r="HL31" s="12"/>
+      <c r="HM31" s="12"/>
+      <c r="HN31" s="12"/>
+      <c r="HO31" s="12"/>
+      <c r="HP31" s="12"/>
+      <c r="HQ31" s="12"/>
+      <c r="HR31" s="12"/>
+      <c r="HS31" s="12"/>
+      <c r="HT31" s="12"/>
+      <c r="HU31" s="12"/>
+      <c r="HV31" s="12"/>
+      <c r="HW31" s="12"/>
+      <c r="HX31" s="12"/>
+      <c r="HY31" s="12"/>
+      <c r="HZ31" s="12"/>
+      <c r="IA31" s="12"/>
+      <c r="IB31" s="12"/>
+      <c r="IC31" s="12"/>
+      <c r="ID31" s="12"/>
+      <c r="IE31" s="12"/>
+      <c r="IF31" s="12"/>
+      <c r="IG31" s="12"/>
+      <c r="IH31" s="12"/>
+      <c r="II31" s="12"/>
+      <c r="IJ31" s="12"/>
+      <c r="IK31" s="12"/>
+      <c r="IL31" s="12"/>
+      <c r="IM31" s="12"/>
+      <c r="IN31" s="12"/>
+      <c r="IO31" s="12"/>
+      <c r="IP31" s="12"/>
+      <c r="IQ31" s="12"/>
+      <c r="IR31" s="12"/>
+      <c r="IS31" s="12"/>
+      <c r="IT31" s="12"/>
+      <c r="IU31" s="12"/>
+      <c r="IV31" s="12"/>
+      <c r="IW31" s="12"/>
+      <c r="IX31" s="12"/>
+      <c r="IY31" s="12"/>
+      <c r="IZ31" s="12"/>
+      <c r="JA31" s="12"/>
+      <c r="JB31" s="12"/>
+      <c r="JC31" s="12"/>
+      <c r="JD31" s="12"/>
+      <c r="JE31" s="12"/>
+      <c r="JF31" s="12"/>
+      <c r="JG31" s="12"/>
+      <c r="JH31" s="12"/>
+      <c r="JI31" s="12"/>
+      <c r="JJ31" s="12"/>
+      <c r="JK31" s="12"/>
+      <c r="JL31" s="12"/>
+      <c r="JM31" s="12"/>
+      <c r="JN31" s="12"/>
+      <c r="JO31" s="12"/>
+      <c r="JP31" s="12"/>
+      <c r="JQ31" s="12"/>
+      <c r="JR31" s="12"/>
+      <c r="JS31" s="12"/>
+      <c r="JT31" s="12"/>
+      <c r="JU31" s="12"/>
+      <c r="JV31" s="12"/>
+      <c r="JW31" s="12"/>
+      <c r="JX31" s="12"/>
+      <c r="JY31" s="12"/>
+      <c r="JZ31" s="12"/>
+      <c r="KA31" s="12"/>
+      <c r="KB31" s="12"/>
+      <c r="KC31" s="12"/>
+      <c r="KD31" s="12"/>
+      <c r="KE31" s="12"/>
+      <c r="KF31" s="12"/>
+      <c r="KG31" s="12"/>
+      <c r="KH31" s="12"/>
+      <c r="KI31" s="12"/>
+      <c r="KJ31" s="12"/>
+      <c r="KK31" s="12"/>
+      <c r="KL31" s="12"/>
+      <c r="KM31" s="12"/>
+      <c r="KN31" s="12"/>
+      <c r="KO31" s="12"/>
+      <c r="KP31" s="12"/>
+      <c r="KQ31" s="12"/>
+      <c r="KR31" s="12"/>
+      <c r="KS31" s="12"/>
+      <c r="KT31" s="12"/>
+      <c r="KU31" s="12"/>
+      <c r="KV31" s="12"/>
+      <c r="KW31" s="12"/>
+      <c r="KX31" s="12"/>
+      <c r="KY31" s="12"/>
+      <c r="KZ31" s="12"/>
+      <c r="LA31" s="12"/>
+      <c r="LB31" s="12"/>
+      <c r="LC31" s="12"/>
+      <c r="LD31" s="12"/>
+      <c r="LE31" s="12"/>
+      <c r="LF31" s="12"/>
+      <c r="LG31" s="12"/>
+      <c r="LH31" s="12"/>
+      <c r="LI31" s="12"/>
+      <c r="LJ31" s="12"/>
+      <c r="LK31" s="12"/>
+      <c r="LL31" s="12"/>
+      <c r="LM31" s="12"/>
+      <c r="LN31" s="12"/>
+      <c r="LO31" s="12"/>
+      <c r="LP31" s="12"/>
+      <c r="LQ31" s="12"/>
+      <c r="LR31" s="12"/>
+      <c r="LS31" s="12"/>
+      <c r="LT31" s="12"/>
+      <c r="LU31" s="12"/>
+      <c r="LV31" s="12"/>
+      <c r="LW31" s="12"/>
+      <c r="LX31" s="12"/>
+      <c r="LY31" s="12"/>
+      <c r="LZ31" s="12"/>
+      <c r="MA31" s="12"/>
+      <c r="MB31" s="12"/>
+      <c r="MC31" s="12"/>
+      <c r="MD31" s="12"/>
+      <c r="ME31" s="12"/>
+      <c r="MF31" s="12"/>
+      <c r="MG31" s="12"/>
+      <c r="MH31" s="12"/>
+      <c r="MI31" s="12"/>
+      <c r="MJ31" s="12"/>
+      <c r="MK31" s="12"/>
+      <c r="ML31" s="12"/>
+      <c r="MM31" s="12"/>
+      <c r="MN31" s="12"/>
+      <c r="MO31" s="12"/>
+      <c r="MP31" s="12"/>
+      <c r="MQ31" s="12"/>
+      <c r="MR31" s="12"/>
+      <c r="MS31" s="12"/>
+      <c r="MT31" s="12"/>
+      <c r="MU31" s="12"/>
+      <c r="MV31" s="12"/>
+      <c r="MW31" s="12"/>
+      <c r="MX31" s="12"/>
+      <c r="MY31" s="12"/>
+      <c r="MZ31" s="12"/>
+      <c r="NA31" s="12"/>
+      <c r="NB31" s="12"/>
+      <c r="NC31" s="12"/>
+      <c r="ND31" s="12"/>
+      <c r="NE31" s="12"/>
+      <c r="NF31" s="12"/>
+      <c r="NG31" s="12"/>
+      <c r="NH31" s="12"/>
+      <c r="NI31" s="12"/>
+      <c r="NJ31" s="12"/>
+      <c r="NK31" s="12"/>
+      <c r="NL31" s="12"/>
+      <c r="NM31" s="12"/>
+      <c r="NN31" s="12"/>
+      <c r="NO31" s="12"/>
+      <c r="NP31" s="12"/>
+      <c r="NQ31" s="12"/>
+      <c r="NR31" s="12"/>
+      <c r="NS31" s="12"/>
+      <c r="NT31" s="12"/>
+      <c r="NU31" s="12"/>
+      <c r="NV31" s="12"/>
+      <c r="NW31" s="12"/>
+      <c r="NX31" s="12"/>
+      <c r="NY31" s="12"/>
+      <c r="NZ31" s="12"/>
+      <c r="OA31" s="12"/>
+      <c r="OB31" s="12"/>
+      <c r="OC31" s="12"/>
+      <c r="OD31" s="12"/>
+      <c r="OE31" s="12"/>
+      <c r="OF31" s="12"/>
+      <c r="OG31" s="12"/>
+      <c r="OH31" s="12"/>
+      <c r="OI31" s="12"/>
+      <c r="OJ31" s="12"/>
+      <c r="OK31" s="12"/>
+      <c r="OL31" s="12"/>
+      <c r="OM31" s="12"/>
+      <c r="ON31" s="12"/>
+      <c r="OO31" s="12"/>
+      <c r="OP31" s="12"/>
+      <c r="OQ31" s="12"/>
+      <c r="OR31" s="12"/>
+      <c r="OS31" s="12"/>
+      <c r="OT31" s="12"/>
+      <c r="OU31" s="12"/>
+      <c r="OV31" s="12"/>
+      <c r="OW31" s="12"/>
+      <c r="OX31" s="12"/>
+      <c r="OY31" s="12"/>
+      <c r="OZ31" s="12"/>
+      <c r="PA31" s="12"/>
+      <c r="PB31" s="12"/>
+      <c r="PC31" s="12"/>
+      <c r="PD31" s="12"/>
+      <c r="PE31" s="12"/>
+      <c r="PF31" s="12"/>
+      <c r="PG31" s="12"/>
+      <c r="PH31" s="12"/>
+      <c r="PI31" s="12"/>
+      <c r="PJ31" s="12"/>
+      <c r="PK31" s="12"/>
+      <c r="PL31" s="12"/>
+      <c r="PM31" s="12"/>
+      <c r="PN31" s="12"/>
+      <c r="PO31" s="12"/>
+      <c r="PP31" s="12"/>
+      <c r="PQ31" s="12"/>
+      <c r="PR31" s="12"/>
+      <c r="PS31" s="12"/>
+      <c r="PT31" s="12"/>
+      <c r="PU31" s="12"/>
+      <c r="PV31" s="12"/>
+      <c r="PW31" s="12"/>
+      <c r="PX31" s="12"/>
+      <c r="PY31" s="12"/>
+      <c r="PZ31" s="12"/>
+      <c r="QA31" s="12"/>
+      <c r="QB31" s="12"/>
+      <c r="QC31" s="12"/>
+      <c r="QD31" s="12"/>
+      <c r="QE31" s="12"/>
+      <c r="QF31" s="12"/>
+      <c r="QG31" s="12"/>
+      <c r="QH31" s="12"/>
+      <c r="QI31" s="12"/>
+      <c r="QJ31" s="12"/>
+      <c r="QK31" s="12"/>
+      <c r="QL31" s="12"/>
+      <c r="QM31" s="12"/>
+      <c r="QN31" s="12"/>
+      <c r="QO31" s="12"/>
+      <c r="QP31" s="12"/>
+      <c r="QQ31" s="12"/>
+      <c r="QR31" s="12"/>
+      <c r="QS31" s="12"/>
+      <c r="QT31" s="12"/>
+      <c r="QU31" s="12"/>
+      <c r="QV31" s="12"/>
+      <c r="QW31" s="12"/>
+      <c r="QX31" s="12"/>
+      <c r="QY31" s="12"/>
+      <c r="QZ31" s="12"/>
+      <c r="RA31" s="12"/>
+      <c r="RB31" s="12"/>
+      <c r="RC31" s="12"/>
+      <c r="RD31" s="12"/>
+      <c r="RE31" s="12"/>
+      <c r="RF31" s="12"/>
+      <c r="RG31" s="12"/>
+      <c r="RH31" s="12"/>
+      <c r="RI31" s="12"/>
+      <c r="RJ31" s="12"/>
+      <c r="RK31" s="12"/>
+      <c r="RL31" s="12"/>
+      <c r="RM31" s="12"/>
+      <c r="RN31" s="12"/>
+      <c r="RO31" s="12"/>
+      <c r="RP31" s="12"/>
+      <c r="RQ31" s="12"/>
+      <c r="RR31" s="12"/>
+      <c r="RS31" s="12"/>
+      <c r="RT31" s="12"/>
+      <c r="RU31" s="12"/>
+      <c r="RV31" s="12"/>
+      <c r="RW31" s="12"/>
+      <c r="RX31" s="12"/>
+      <c r="RY31" s="12"/>
+      <c r="RZ31" s="12"/>
+      <c r="SA31" s="12"/>
+      <c r="SB31" s="12"/>
+      <c r="SC31" s="12"/>
+      <c r="SD31" s="12"/>
+      <c r="SE31" s="12"/>
+      <c r="SF31" s="12"/>
+      <c r="SG31" s="12"/>
+      <c r="SH31" s="12"/>
+      <c r="SI31" s="12"/>
+      <c r="SJ31" s="12"/>
+      <c r="SK31" s="12"/>
+      <c r="SL31" s="12"/>
+      <c r="SM31" s="12"/>
+      <c r="SN31" s="12"/>
+      <c r="SO31" s="12"/>
+      <c r="SP31" s="12"/>
+      <c r="SQ31" s="12"/>
+      <c r="SR31" s="12"/>
+      <c r="SS31" s="12"/>
+      <c r="ST31" s="12"/>
+      <c r="SU31" s="12"/>
+      <c r="SV31" s="12"/>
+      <c r="SW31" s="12"/>
+      <c r="SX31" s="12"/>
+      <c r="SY31" s="12"/>
+      <c r="SZ31" s="12"/>
+      <c r="TA31" s="12"/>
+      <c r="TB31" s="12"/>
+      <c r="TC31" s="12"/>
+      <c r="TD31" s="12"/>
+      <c r="TE31" s="12"/>
+      <c r="TF31" s="12"/>
+      <c r="TG31" s="12"/>
+      <c r="TH31" s="12"/>
+      <c r="TI31" s="12"/>
+      <c r="TJ31" s="12"/>
+      <c r="TK31" s="12"/>
+      <c r="TL31" s="12"/>
+      <c r="TM31" s="12"/>
+      <c r="TN31" s="12"/>
+      <c r="TO31" s="12"/>
+      <c r="TP31" s="12"/>
+      <c r="TQ31" s="12"/>
+      <c r="TR31" s="12"/>
+      <c r="TS31" s="12"/>
+      <c r="TT31" s="12"/>
+      <c r="TU31" s="12"/>
+      <c r="TV31" s="12"/>
+      <c r="TW31" s="12"/>
+      <c r="TX31" s="12"/>
+      <c r="TY31" s="12"/>
+      <c r="TZ31" s="12"/>
+      <c r="UA31" s="12"/>
+      <c r="UB31" s="12"/>
+      <c r="UC31" s="12"/>
+      <c r="UD31" s="12"/>
+      <c r="UE31" s="12"/>
+      <c r="UF31" s="12"/>
+      <c r="UG31" s="12"/>
+      <c r="UH31" s="12"/>
+      <c r="UI31" s="12"/>
+      <c r="UJ31" s="12"/>
+      <c r="UK31" s="12"/>
+      <c r="UL31" s="12"/>
+      <c r="UM31" s="12"/>
+      <c r="UN31" s="12"/>
+      <c r="UO31" s="12"/>
+      <c r="UP31" s="12"/>
+      <c r="UQ31" s="12"/>
+      <c r="UR31" s="12"/>
+      <c r="US31" s="12"/>
+      <c r="UT31" s="12"/>
+      <c r="UU31" s="12"/>
+      <c r="UV31" s="12"/>
+      <c r="UW31" s="12"/>
+      <c r="UX31" s="12"/>
+      <c r="UY31" s="12"/>
+      <c r="UZ31" s="12"/>
+      <c r="VA31" s="12"/>
+      <c r="VB31" s="12"/>
+      <c r="VC31" s="12"/>
+      <c r="VD31" s="12"/>
+      <c r="VE31" s="12"/>
+      <c r="VF31" s="12"/>
+      <c r="VG31" s="12"/>
+      <c r="VH31" s="12"/>
+      <c r="VI31" s="12"/>
+      <c r="VJ31" s="12"/>
+      <c r="VK31" s="12"/>
+      <c r="VL31" s="12"/>
+      <c r="VM31" s="12"/>
+      <c r="VN31" s="12"/>
+      <c r="VO31" s="12"/>
+      <c r="VP31" s="12"/>
+      <c r="VQ31" s="12"/>
+      <c r="VR31" s="12"/>
+      <c r="VS31" s="12"/>
+      <c r="VT31" s="12"/>
+      <c r="VU31" s="12"/>
+      <c r="VV31" s="12"/>
+      <c r="VW31" s="12"/>
+      <c r="VX31" s="12"/>
+      <c r="VY31" s="12"/>
+      <c r="VZ31" s="12"/>
+      <c r="WA31" s="12"/>
+      <c r="WB31" s="12"/>
+      <c r="WC31" s="12"/>
+      <c r="WD31" s="12"/>
+      <c r="WE31" s="12"/>
+      <c r="WF31" s="12"/>
+      <c r="WG31" s="12"/>
+      <c r="WH31" s="12"/>
+      <c r="WI31" s="12"/>
+      <c r="WJ31" s="12"/>
+      <c r="WK31" s="12"/>
+      <c r="WL31" s="12"/>
+      <c r="WM31" s="12"/>
+      <c r="WN31" s="12"/>
+      <c r="WO31" s="12"/>
+      <c r="WP31" s="12"/>
+      <c r="WQ31" s="12"/>
+      <c r="WR31" s="12"/>
+      <c r="WS31" s="12"/>
+      <c r="WT31" s="12"/>
+      <c r="WU31" s="12"/>
+      <c r="WV31" s="12"/>
+      <c r="WW31" s="12"/>
+      <c r="WX31" s="12"/>
+      <c r="WY31" s="12"/>
+      <c r="WZ31" s="12"/>
+      <c r="XA31" s="12"/>
+      <c r="XB31" s="12"/>
+      <c r="XC31" s="12"/>
+      <c r="XD31" s="12"/>
+      <c r="XE31" s="12"/>
+      <c r="XF31" s="12"/>
+      <c r="XG31" s="12"/>
+      <c r="XH31" s="12"/>
+      <c r="XI31" s="12"/>
+      <c r="XJ31" s="12"/>
+      <c r="XK31" s="12"/>
+      <c r="XL31" s="12"/>
+      <c r="XM31" s="12"/>
+      <c r="XN31" s="12"/>
+      <c r="XO31" s="12"/>
+      <c r="XP31" s="12"/>
+      <c r="XQ31" s="12"/>
+      <c r="XR31" s="12"/>
+      <c r="XS31" s="12"/>
+      <c r="XT31" s="12"/>
+      <c r="XU31" s="12"/>
+      <c r="XV31" s="12"/>
+      <c r="XW31" s="12"/>
+      <c r="XX31" s="12"/>
+      <c r="XY31" s="12"/>
+      <c r="XZ31" s="12"/>
+      <c r="YA31" s="12"/>
+      <c r="YB31" s="12"/>
+      <c r="YC31" s="12"/>
+      <c r="YD31" s="12"/>
+      <c r="YE31" s="12"/>
+      <c r="YF31" s="12"/>
+      <c r="YG31" s="12"/>
+      <c r="YH31" s="12"/>
+      <c r="YI31" s="12"/>
+      <c r="YJ31" s="12"/>
+      <c r="YK31" s="12"/>
+      <c r="YL31" s="12"/>
+      <c r="YM31" s="12"/>
+      <c r="YN31" s="12"/>
+      <c r="YO31" s="12"/>
+      <c r="YP31" s="12"/>
+      <c r="YQ31" s="12"/>
+      <c r="YR31" s="12"/>
+      <c r="YS31" s="12"/>
+      <c r="YT31" s="12"/>
+      <c r="YU31" s="12"/>
+      <c r="YV31" s="12"/>
+      <c r="YW31" s="12"/>
+      <c r="YX31" s="12"/>
+      <c r="YY31" s="12"/>
+      <c r="YZ31" s="12"/>
+      <c r="ZA31" s="12"/>
+      <c r="ZB31" s="12"/>
+      <c r="ZC31" s="12"/>
+      <c r="ZD31" s="12"/>
+      <c r="ZE31" s="12"/>
+      <c r="ZF31" s="12"/>
+      <c r="ZG31" s="12"/>
+      <c r="ZH31" s="12"/>
+      <c r="ZI31" s="12"/>
+      <c r="ZJ31" s="12"/>
+      <c r="ZK31" s="12"/>
+      <c r="ZL31" s="12"/>
+      <c r="ZM31" s="12"/>
+      <c r="ZN31" s="12"/>
+      <c r="ZO31" s="12"/>
+      <c r="ZP31" s="12"/>
+      <c r="ZQ31" s="12"/>
+      <c r="ZR31" s="12"/>
+      <c r="ZS31" s="12"/>
+      <c r="ZT31" s="12"/>
+      <c r="ZU31" s="12"/>
+      <c r="ZV31" s="12"/>
+      <c r="ZW31" s="12"/>
+      <c r="ZX31" s="12"/>
+      <c r="ZY31" s="12"/>
+      <c r="ZZ31" s="12"/>
+      <c r="AAA31" s="12"/>
+      <c r="AAB31" s="12"/>
+      <c r="AAC31" s="12"/>
+      <c r="AAD31" s="12"/>
+      <c r="AAE31" s="12"/>
+      <c r="AAF31" s="12"/>
+      <c r="AAG31" s="12"/>
+      <c r="AAH31" s="12"/>
+      <c r="AAI31" s="12"/>
+      <c r="AAJ31" s="12"/>
+      <c r="AAK31" s="12"/>
+      <c r="AAL31" s="12"/>
+      <c r="AAM31" s="12"/>
+      <c r="AAN31" s="12"/>
+      <c r="AAO31" s="12"/>
+      <c r="AAP31" s="12"/>
+      <c r="AAQ31" s="12"/>
+      <c r="AAR31" s="12"/>
+      <c r="AAS31" s="12"/>
+      <c r="AAT31" s="12"/>
+      <c r="AAU31" s="12"/>
+      <c r="AAV31" s="12"/>
+      <c r="AAW31" s="12"/>
+      <c r="AAX31" s="12"/>
+      <c r="AAY31" s="12"/>
+      <c r="AAZ31" s="12"/>
+      <c r="ABA31" s="12"/>
+      <c r="ABB31" s="12"/>
+      <c r="ABC31" s="12"/>
+      <c r="ABD31" s="12"/>
+      <c r="ABE31" s="12"/>
+      <c r="ABF31" s="12"/>
+      <c r="ABG31" s="12"/>
+      <c r="ABH31" s="12"/>
+      <c r="ABI31" s="12"/>
+      <c r="ABJ31" s="12"/>
+      <c r="ABK31" s="12"/>
+      <c r="ABL31" s="12"/>
+      <c r="ABM31" s="12"/>
+      <c r="ABN31" s="12"/>
+      <c r="ABO31" s="12"/>
+      <c r="ABP31" s="12"/>
+      <c r="ABQ31" s="12"/>
+      <c r="ABR31" s="12"/>
+      <c r="ABS31" s="12"/>
+      <c r="ABT31" s="12"/>
+      <c r="ABU31" s="12"/>
+      <c r="ABV31" s="12"/>
+      <c r="ABW31" s="12"/>
+      <c r="ABX31" s="12"/>
+      <c r="ABY31" s="12"/>
+      <c r="ABZ31" s="12"/>
+      <c r="ACA31" s="12"/>
+      <c r="ACB31" s="12"/>
+      <c r="ACC31" s="12"/>
+      <c r="ACD31" s="12"/>
+      <c r="ACE31" s="12"/>
+      <c r="ACF31" s="12"/>
+      <c r="ACG31" s="12"/>
+      <c r="ACH31" s="12"/>
+      <c r="ACI31" s="12"/>
+      <c r="ACJ31" s="12"/>
+      <c r="ACK31" s="12"/>
+      <c r="ACL31" s="12"/>
+      <c r="ACM31" s="12"/>
+      <c r="ACN31" s="12"/>
+      <c r="ACO31" s="12"/>
+      <c r="ACP31" s="12"/>
+      <c r="ACQ31" s="12"/>
+      <c r="ACR31" s="12"/>
+      <c r="ACS31" s="12"/>
+      <c r="ACT31" s="12"/>
+      <c r="ACU31" s="12"/>
+      <c r="ACV31" s="12"/>
+      <c r="ACW31" s="12"/>
+      <c r="ACX31" s="12"/>
+      <c r="ACY31" s="12"/>
+      <c r="ACZ31" s="12"/>
+      <c r="ADA31" s="12"/>
+      <c r="ADB31" s="12"/>
+      <c r="ADC31" s="12"/>
+      <c r="ADD31" s="12"/>
+      <c r="ADE31" s="12"/>
+      <c r="ADF31" s="12"/>
+      <c r="ADG31" s="12"/>
+      <c r="ADH31" s="12"/>
+      <c r="ADI31" s="12"/>
+      <c r="ADJ31" s="12"/>
+      <c r="ADK31" s="12"/>
+      <c r="ADL31" s="12"/>
+      <c r="ADM31" s="12"/>
+      <c r="ADN31" s="12"/>
+      <c r="ADO31" s="12"/>
+      <c r="ADP31" s="12"/>
+      <c r="ADQ31" s="12"/>
+      <c r="ADR31" s="12"/>
+      <c r="ADS31" s="12"/>
+      <c r="ADT31" s="12"/>
+      <c r="ADU31" s="12"/>
+      <c r="ADV31" s="12"/>
+      <c r="ADW31" s="12"/>
+      <c r="ADX31" s="12"/>
+      <c r="ADY31" s="12"/>
+      <c r="ADZ31" s="12"/>
+      <c r="AEA31" s="12"/>
+      <c r="AEB31" s="12"/>
+      <c r="AEC31" s="12"/>
+      <c r="AED31" s="12"/>
+      <c r="AEE31" s="12"/>
+      <c r="AEF31" s="12"/>
+      <c r="AEG31" s="12"/>
+      <c r="AEH31" s="12"/>
+      <c r="AEI31" s="12"/>
+      <c r="AEJ31" s="12"/>
+      <c r="AEK31" s="12"/>
+      <c r="AEL31" s="12"/>
+      <c r="AEM31" s="12"/>
+      <c r="AEN31" s="12"/>
+      <c r="AEO31" s="12"/>
+      <c r="AEP31" s="12"/>
+      <c r="AEQ31" s="12"/>
+      <c r="AER31" s="12"/>
+      <c r="AES31" s="12"/>
+      <c r="AET31" s="12"/>
+      <c r="AEU31" s="12"/>
+      <c r="AEV31" s="12"/>
+      <c r="AEW31" s="12"/>
+      <c r="AEX31" s="12"/>
+      <c r="AEY31" s="12"/>
+      <c r="AEZ31" s="12"/>
+      <c r="AFA31" s="12"/>
+      <c r="AFB31" s="12"/>
+      <c r="AFC31" s="12"/>
+      <c r="AFD31" s="12"/>
+      <c r="AFE31" s="12"/>
+      <c r="AFF31" s="12"/>
+      <c r="AFG31" s="12"/>
+      <c r="AFH31" s="12"/>
+      <c r="AFI31" s="12"/>
+      <c r="AFJ31" s="12"/>
+      <c r="AFK31" s="12"/>
+      <c r="AFL31" s="12"/>
+      <c r="AFM31" s="12"/>
+      <c r="AFN31" s="12"/>
+      <c r="AFO31" s="12"/>
+      <c r="AFP31" s="12"/>
+      <c r="AFQ31" s="12"/>
+      <c r="AFR31" s="12"/>
+      <c r="AFS31" s="12"/>
+      <c r="AFT31" s="12"/>
+      <c r="AFU31" s="12"/>
+      <c r="AFV31" s="12"/>
+      <c r="AFW31" s="12"/>
+      <c r="AFX31" s="12"/>
+      <c r="AFY31" s="12"/>
+      <c r="AFZ31" s="12"/>
+      <c r="AGA31" s="12"/>
+      <c r="AGB31" s="12"/>
+      <c r="AGC31" s="12"/>
+      <c r="AGD31" s="12"/>
+      <c r="AGE31" s="12"/>
+      <c r="AGF31" s="12"/>
+      <c r="AGG31" s="12"/>
+      <c r="AGH31" s="12"/>
+      <c r="AGI31" s="12"/>
+      <c r="AGJ31" s="12"/>
+      <c r="AGK31" s="12"/>
+      <c r="AGL31" s="12"/>
+      <c r="AGM31" s="12"/>
+      <c r="AGN31" s="12"/>
+      <c r="AGO31" s="12"/>
+      <c r="AGP31" s="12"/>
+      <c r="AGQ31" s="12"/>
+      <c r="AGR31" s="12"/>
+      <c r="AGS31" s="12"/>
+      <c r="AGT31" s="12"/>
+      <c r="AGU31" s="12"/>
+      <c r="AGV31" s="12"/>
+      <c r="AGW31" s="12"/>
+      <c r="AGX31" s="12"/>
+      <c r="AGY31" s="12"/>
+      <c r="AGZ31" s="12"/>
+      <c r="AHA31" s="12"/>
+      <c r="AHB31" s="12"/>
+      <c r="AHC31" s="12"/>
+      <c r="AHD31" s="12"/>
+      <c r="AHE31" s="12"/>
+      <c r="AHF31" s="12"/>
+      <c r="AHG31" s="12"/>
+      <c r="AHH31" s="12"/>
+      <c r="AHI31" s="12"/>
+      <c r="AHJ31" s="12"/>
+      <c r="AHK31" s="12"/>
+      <c r="AHL31" s="12"/>
+      <c r="AHM31" s="12"/>
+      <c r="AHN31" s="12"/>
+      <c r="AHO31" s="12"/>
+      <c r="AHP31" s="12"/>
+      <c r="AHQ31" s="12"/>
+      <c r="AHR31" s="12"/>
+      <c r="AHS31" s="12"/>
+      <c r="AHT31" s="12"/>
+      <c r="AHU31" s="12"/>
+      <c r="AHV31" s="12"/>
+      <c r="AHW31" s="12"/>
+      <c r="AHX31" s="12"/>
+      <c r="AHY31" s="12"/>
+      <c r="AHZ31" s="12"/>
+      <c r="AIA31" s="12"/>
+      <c r="AIB31" s="12"/>
+      <c r="AIC31" s="12"/>
+      <c r="AID31" s="12"/>
+      <c r="AIE31" s="12"/>
+      <c r="AIF31" s="12"/>
+      <c r="AIG31" s="12"/>
+      <c r="AIH31" s="12"/>
+      <c r="AII31" s="12"/>
+      <c r="AIJ31" s="12"/>
+      <c r="AIK31" s="12"/>
+      <c r="AIL31" s="12"/>
+      <c r="AIM31" s="12"/>
+      <c r="AIN31" s="12"/>
+      <c r="AIO31" s="12"/>
+      <c r="AIP31" s="12"/>
+      <c r="AIQ31" s="12"/>
+      <c r="AIR31" s="12"/>
+      <c r="AIS31" s="12"/>
+      <c r="AIT31" s="12"/>
+      <c r="AIU31" s="12"/>
+      <c r="AIV31" s="12"/>
+      <c r="AIW31" s="12"/>
+      <c r="AIX31" s="12"/>
+      <c r="AIY31" s="12"/>
+      <c r="AIZ31" s="12"/>
+      <c r="AJA31" s="12"/>
+      <c r="AJB31" s="12"/>
+      <c r="AJC31" s="12"/>
+      <c r="AJD31" s="12"/>
+      <c r="AJE31" s="12"/>
+      <c r="AJF31" s="12"/>
+      <c r="AJG31" s="12"/>
+      <c r="AJH31" s="12"/>
+      <c r="AJI31" s="12"/>
+      <c r="AJJ31" s="12"/>
+      <c r="AJK31" s="12"/>
+      <c r="AJL31" s="12"/>
+      <c r="AJM31" s="12"/>
+      <c r="AJN31" s="12"/>
+      <c r="AJO31" s="12"/>
+      <c r="AJP31" s="12"/>
+      <c r="AJQ31" s="12"/>
+      <c r="AJR31" s="12"/>
+      <c r="AJS31" s="12"/>
+      <c r="AJT31" s="12"/>
+      <c r="AJU31" s="12"/>
+      <c r="AJV31" s="12"/>
+      <c r="AJW31" s="12"/>
+      <c r="AJX31" s="12"/>
+      <c r="AJY31" s="12"/>
+      <c r="AJZ31" s="12"/>
+      <c r="AKA31" s="12"/>
+      <c r="AKB31" s="12"/>
+      <c r="AKC31" s="12"/>
+      <c r="AKD31" s="12"/>
+      <c r="AKE31" s="12"/>
+      <c r="AKF31" s="12"/>
+      <c r="AKG31" s="12"/>
+      <c r="AKH31" s="12"/>
+      <c r="AKI31" s="12"/>
+      <c r="AKJ31" s="12"/>
+      <c r="AKK31" s="12"/>
+      <c r="AKL31" s="12"/>
+      <c r="AKM31" s="12"/>
+      <c r="AKN31" s="12"/>
+      <c r="AKO31" s="12"/>
+      <c r="AKP31" s="12"/>
+      <c r="AKQ31" s="12"/>
+      <c r="AKR31" s="12"/>
+      <c r="AKS31" s="12"/>
+      <c r="AKT31" s="12"/>
+      <c r="AKU31" s="12"/>
+      <c r="AKV31" s="12"/>
+      <c r="AKW31" s="12"/>
+      <c r="AKX31" s="12"/>
+      <c r="AKY31" s="12"/>
+      <c r="AKZ31" s="12"/>
+      <c r="ALA31" s="12"/>
+      <c r="ALB31" s="12"/>
+      <c r="ALC31" s="12"/>
+      <c r="ALD31" s="12"/>
+      <c r="ALE31" s="12"/>
+      <c r="ALF31" s="12"/>
+      <c r="ALG31" s="12"/>
+      <c r="ALH31" s="12"/>
+      <c r="ALI31" s="12"/>
+      <c r="ALJ31" s="12"/>
+      <c r="ALK31" s="12"/>
+      <c r="ALL31" s="12"/>
+      <c r="ALM31" s="12"/>
+      <c r="ALN31" s="12"/>
+      <c r="ALO31" s="12"/>
+      <c r="ALP31" s="12"/>
+      <c r="ALQ31" s="12"/>
+      <c r="ALR31" s="12"/>
+      <c r="ALS31" s="12"/>
+      <c r="ALT31" s="12"/>
+      <c r="ALU31" s="12"/>
+      <c r="ALV31" s="12"/>
+      <c r="ALW31" s="12"/>
+      <c r="ALX31" s="12"/>
+      <c r="ALY31" s="12"/>
+      <c r="ALZ31" s="12"/>
+      <c r="AMA31" s="12"/>
+      <c r="AMB31" s="12"/>
+      <c r="AMC31" s="12"/>
+      <c r="AMD31" s="12"/>
+      <c r="AME31" s="12"/>
+      <c r="AMF31" s="12"/>
+      <c r="AMG31" s="12"/>
+      <c r="AMH31" s="12"/>
+      <c r="AMI31" s="12"/>
+      <c r="AMJ31" s="12"/>
+      <c r="AMK31" s="12"/>
+      <c r="AML31" s="12"/>
+      <c r="AMM31" s="12"/>
+    </row>
+    <row r="32" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>16</v>
@@ -4437,28 +6576,31 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K32" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>461</v>
+      <c r="I32" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>16</v>
@@ -4468,24 +6610,27 @@
         <v>0</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>16</v>
@@ -4495,27 +6640,27 @@
         <v>0</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="L34" s="13" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="285" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>16</v>
@@ -4525,30 +6670,24 @@
         <v>0</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="L35" s="13" t="s">
-        <v>463</v>
+        <v>137</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>16</v>
@@ -4557,64 +6696,61 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="I36" s="8" t="s">
-        <v>103</v>
+      <c r="K36" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="L36" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="285" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>347</v>
+        <v>147</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G37" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>153</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>158</v>
+        <v>406</v>
       </c>
       <c r="L37" s="13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>16</v>
@@ -4623,24 +6759,32 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
+      <c r="I38" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="L38" s="13" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E39" s="9"/>
+        <v>347</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="F39" s="1" t="s">
         <v>16</v>
       </c>
@@ -4651,31 +6795,28 @@
       <c r="H39" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I39" s="8" t="s">
-        <v>162</v>
+      <c r="K39" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>466</v>
-      </c>
-      <c r="M39" s="12" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>16</v>
@@ -4684,48 +6825,60 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M40" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="L40" s="13" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>168</v>
+        <v>38</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>169</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="E41" s="9"/>
       <c r="F41" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G41" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="L41" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="M41" s="12" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>168</v>
+        <v>38</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E42" s="9"/>
+        <v>165</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="F42" s="1" t="s">
         <v>16</v>
       </c>
@@ -4733,241 +6886,246 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K42" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="L42" s="13" t="s">
-        <v>467</v>
-      </c>
       <c r="M42" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>168</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G43" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E44" s="9"/>
+      <c r="F44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="L44" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="46" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G44" s="7" t="b">
+      <c r="G46" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="I46" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="J46" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="L44" s="13" t="s">
+      <c r="L46" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="M46" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="47" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D47" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="G45" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I45" s="8" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E46" s="9"/>
-      <c r="F46" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G46" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I46" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="G47" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="I47" s="8" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>54</v>
+        <v>168</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>182</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="E48" s="9"/>
       <c r="F48" s="1" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="G48" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>363</v>
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>190</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
-        <v>196</v>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E49" s="9"/>
+        <v>178</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="F49" s="1" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="G49" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>200</v>
+    <row r="50" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>202</v>
+        <v>54</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E50" s="9"/>
+        <v>182</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="F50" s="1" t="s">
         <v>153</v>
       </c>
       <c r="G50" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E51" s="9"/>
       <c r="F51" s="1" t="s">
@@ -4978,18 +7136,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>106</v>
+        <v>202</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E52" s="9"/>
       <c r="F52" s="1" t="s">
@@ -5000,18 +7158,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E53" s="9"/>
       <c r="F53" s="1" t="s">
@@ -5022,18 +7180,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>217</v>
+        <v>106</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="1" t="s">
@@ -5044,19 +7202,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>222</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="E55" s="9"/>
       <c r="F55" s="1" t="s">
         <v>153</v>
       </c>
@@ -5065,18 +7224,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E56" s="9"/>
       <c r="F56" s="1" t="s">
@@ -5087,20 +7246,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E57" s="9"/>
+        <v>222</v>
+      </c>
       <c r="F57" s="1" t="s">
         <v>153</v>
       </c>
@@ -5109,18 +7267,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>95</v>
+        <v>225</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E58" s="9"/>
       <c r="F58" s="1" t="s">
@@ -5131,18 +7289,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
-        <v>234</v>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>227</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="E59" s="9"/>
       <c r="F59" s="1" t="s">
@@ -5153,18 +7311,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>238</v>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>231</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>240</v>
+        <v>95</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="1" t="s">
@@ -5175,18 +7333,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E61" s="9"/>
       <c r="F61" s="1" t="s">
@@ -5197,18 +7355,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E62" s="9"/>
       <c r="F62" s="1" t="s">
@@ -5219,18 +7377,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E63" s="9"/>
       <c r="F63" s="1" t="s">
@@ -5241,18 +7399,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>123</v>
+        <v>248</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="E64" s="9"/>
       <c r="F64" s="1" t="s">
@@ -5265,16 +7423,16 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E65" s="9"/>
       <c r="F65" s="1" t="s">
@@ -5287,16 +7445,16 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>263</v>
+        <v>123</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="E66" s="9"/>
       <c r="F66" s="1" t="s">
@@ -5309,16 +7467,16 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="E67" s="9"/>
       <c r="F67" s="1" t="s">
@@ -5331,16 +7489,16 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="E68" s="9"/>
       <c r="F68" s="1" t="s">
@@ -5351,18 +7509,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="E69" s="9"/>
       <c r="F69" s="1" t="s">
@@ -5375,16 +7533,16 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E70" s="9"/>
       <c r="F70" s="1" t="s">
@@ -5395,18 +7553,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>58</v>
+        <v>275</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="E71" s="9"/>
       <c r="F71" s="1" t="s">
@@ -5419,16 +7577,16 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E72" s="9"/>
       <c r="F72" s="1" t="s">
@@ -5441,16 +7599,16 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>290</v>
+        <v>58</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="1" t="s">
@@ -5463,16 +7621,16 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E74" s="9"/>
       <c r="F74" s="1" t="s">
@@ -5485,16 +7643,16 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="E75" s="9"/>
       <c r="F75" s="1" t="s">
@@ -5507,16 +7665,16 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="1" t="s">
@@ -5529,16 +7687,16 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="E77" s="9"/>
       <c r="F77" s="1" t="s">
@@ -5551,17 +7709,18 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>311</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="E78" s="9"/>
       <c r="F78" s="1" t="s">
         <v>153</v>
       </c>
@@ -5572,16 +7731,16 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="E79" s="9"/>
       <c r="F79" s="1" t="s">
@@ -5592,20 +7751,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="E80" s="9"/>
+        <v>311</v>
+      </c>
       <c r="F80" s="1" t="s">
         <v>153</v>
       </c>
@@ -5615,139 +7773,183 @@
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>320</v>
+      <c r="A81" s="11" t="s">
+        <v>312</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>58</v>
+        <v>314</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>322</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="E81" s="9"/>
       <c r="F81" s="1" t="s">
-        <v>323</v>
+        <v>153</v>
       </c>
       <c r="G81" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M81" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>325</v>
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="11" t="s">
+        <v>316</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>20</v>
+        <v>318</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>327</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="E82" s="9"/>
       <c r="F82" s="1" t="s">
-        <v>328</v>
+        <v>153</v>
       </c>
       <c r="G82" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>87</v>
+        <v>323</v>
       </c>
       <c r="G83" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="I83" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="K83" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="L83" s="13" t="s">
-        <v>468</v>
+        <v>92</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>87</v>
+        <v>328</v>
       </c>
       <c r="G84" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>229</v>
+        <v>106</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>339</v>
+        <v>331</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>332</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G85" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H85" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="I85" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="L85" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G86" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G87" s="7" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H87" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="M85" s="1" t="s">
+      <c r="M87" s="1" t="s">
         <v>429</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M85" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M87" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added 0212 and 0213; TICC-170
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Participant identifier schemes v7.5.xlsx
+++ b/work-in-progress/Peppol Code Lists - Participant identifier schemes v7.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472BF571-7439-4E9F-BAAE-8616315DE727}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072B0D12-54D6-4D5E-99E3-8DBC86062F35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$M$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Participant Identifier Scheme'!$A$1:$M$89</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
 </workbook>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="501">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -1722,9 +1722,6 @@
     <t>Character Repertoire : A to Z (upper case) and 0 to 9</t>
   </si>
   <si>
-    <t>Codice fiscale is the Italian tax identification number and is the code that serves to unambiguously identify individuals or subjects other than natural persons residing in Italy. Designed by and for the Italian tax Agency, it is now used for several other purposes, e.g. uniquely identifying individuals in the health system, or subjects who act as parties in public or private contracts. The code is issued by the Italian tax Agency</t>
-  </si>
-  <si>
     <t>PARTITA IVA</t>
   </si>
   <si>
@@ -1737,7 +1734,47 @@
     <t>Character Repertoire: 0 to 9</t>
   </si>
   <si>
-    <t>VAT registration number is an identifier used for value added tax purposes</t>
+    <t>FI:ORG</t>
+  </si>
+  <si>
+    <t>0212</t>
+  </si>
+  <si>
+    <t>FI:VAT</t>
+  </si>
+  <si>
+    <t>0213</t>
+  </si>
+  <si>
+    <t>Finnish Organization Identifier</t>
+  </si>
+  <si>
+    <t>State Treasury of Finland / Valtiokonttori</t>
+  </si>
+  <si>
+    <t>9999999-9
+nine characters
+last digit after the hyphen is check character</t>
+  </si>
+  <si>
+    <t>Shall be presented as string so that leading zeros have to be present.
+Hyphen shall be present between last two digits.</t>
+  </si>
+  <si>
+    <t>Character Repertoire: digits 0-9 and hyphen "-"</t>
+  </si>
+  <si>
+    <t>Finnish Organization Value Add Tax Identifier</t>
+  </si>
+  <si>
+    <t>FI99999999
+ten characters</t>
+  </si>
+  <si>
+    <t>Shall be presented as string so that leading zeros have to be present. Two first characters have always fixed value FI.</t>
+  </si>
+  <si>
+    <t>Character Repertoire: digits 0-9 and FI</t>
   </si>
 </sst>
 </file>
@@ -2005,6 +2042,60 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01CC2018-35F1-4C40-A115-D838395D8EEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9734550" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1333500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C8DD92B-B6AD-4BE7-89FF-66B2A41F217E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2364,13 +2455,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMM87"/>
+  <dimension ref="A1:AMM89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4455,7 +4546,7 @@
       <c r="AML29" s="12"/>
       <c r="AMM29" s="12"/>
     </row>
-    <row r="30" spans="1:1027" ht="285" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1027" ht="255" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>145</v>
       </c>
@@ -4486,9 +4577,7 @@
       <c r="L30" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="M30" s="12" t="s">
-        <v>485</v>
-      </c>
+      <c r="M30" s="12"/>
       <c r="N30" s="12"/>
       <c r="O30" s="12"/>
       <c r="P30" s="12"/>
@@ -5515,7 +5604,7 @@
         <v>54</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>482</v>
@@ -5529,15 +5618,13 @@
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="8" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K31" s="15"/>
       <c r="L31" s="13" t="s">
-        <v>488</v>
-      </c>
-      <c r="M31" s="12" t="s">
-        <v>489</v>
-      </c>
+        <v>487</v>
+      </c>
+      <c r="M31" s="12"/>
       <c r="N31" s="12"/>
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
@@ -6553,84 +6640,2121 @@
       <c r="AML31" s="12"/>
       <c r="AMM31" s="12"/>
     </row>
-    <row r="32" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>16</v>
+    <row r="32" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>488</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>489</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>492</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>475</v>
       </c>
       <c r="G32" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
+      <c r="H32" s="12"/>
       <c r="I32" s="8" t="s">
-        <v>130</v>
+        <v>494</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>420</v>
-      </c>
+        <v>495</v>
+      </c>
+      <c r="K32" s="15"/>
+      <c r="L32" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+      <c r="W32" s="12"/>
+      <c r="X32" s="12"/>
+      <c r="Y32" s="12"/>
+      <c r="Z32" s="12"/>
+      <c r="AA32" s="12"/>
+      <c r="AB32" s="12"/>
+      <c r="AC32" s="12"/>
+      <c r="AD32" s="12"/>
+      <c r="AE32" s="12"/>
+      <c r="AF32" s="12"/>
+      <c r="AG32" s="12"/>
+      <c r="AH32" s="12"/>
+      <c r="AI32" s="12"/>
+      <c r="AJ32" s="12"/>
+      <c r="AK32" s="12"/>
+      <c r="AL32" s="12"/>
+      <c r="AM32" s="12"/>
+      <c r="AN32" s="12"/>
+      <c r="AO32" s="12"/>
+      <c r="AP32" s="12"/>
+      <c r="AQ32" s="12"/>
+      <c r="AR32" s="12"/>
+      <c r="AS32" s="12"/>
+      <c r="AT32" s="12"/>
+      <c r="AU32" s="12"/>
+      <c r="AV32" s="12"/>
+      <c r="AW32" s="12"/>
+      <c r="AX32" s="12"/>
+      <c r="AY32" s="12"/>
+      <c r="AZ32" s="12"/>
+      <c r="BA32" s="12"/>
+      <c r="BB32" s="12"/>
+      <c r="BC32" s="12"/>
+      <c r="BD32" s="12"/>
+      <c r="BE32" s="12"/>
+      <c r="BF32" s="12"/>
+      <c r="BG32" s="12"/>
+      <c r="BH32" s="12"/>
+      <c r="BI32" s="12"/>
+      <c r="BJ32" s="12"/>
+      <c r="BK32" s="12"/>
+      <c r="BL32" s="12"/>
+      <c r="BM32" s="12"/>
+      <c r="BN32" s="12"/>
+      <c r="BO32" s="12"/>
+      <c r="BP32" s="12"/>
+      <c r="BQ32" s="12"/>
+      <c r="BR32" s="12"/>
+      <c r="BS32" s="12"/>
+      <c r="BT32" s="12"/>
+      <c r="BU32" s="12"/>
+      <c r="BV32" s="12"/>
+      <c r="BW32" s="12"/>
+      <c r="BX32" s="12"/>
+      <c r="BY32" s="12"/>
+      <c r="BZ32" s="12"/>
+      <c r="CA32" s="12"/>
+      <c r="CB32" s="12"/>
+      <c r="CC32" s="12"/>
+      <c r="CD32" s="12"/>
+      <c r="CE32" s="12"/>
+      <c r="CF32" s="12"/>
+      <c r="CG32" s="12"/>
+      <c r="CH32" s="12"/>
+      <c r="CI32" s="12"/>
+      <c r="CJ32" s="12"/>
+      <c r="CK32" s="12"/>
+      <c r="CL32" s="12"/>
+      <c r="CM32" s="12"/>
+      <c r="CN32" s="12"/>
+      <c r="CO32" s="12"/>
+      <c r="CP32" s="12"/>
+      <c r="CQ32" s="12"/>
+      <c r="CR32" s="12"/>
+      <c r="CS32" s="12"/>
+      <c r="CT32" s="12"/>
+      <c r="CU32" s="12"/>
+      <c r="CV32" s="12"/>
+      <c r="CW32" s="12"/>
+      <c r="CX32" s="12"/>
+      <c r="CY32" s="12"/>
+      <c r="CZ32" s="12"/>
+      <c r="DA32" s="12"/>
+      <c r="DB32" s="12"/>
+      <c r="DC32" s="12"/>
+      <c r="DD32" s="12"/>
+      <c r="DE32" s="12"/>
+      <c r="DF32" s="12"/>
+      <c r="DG32" s="12"/>
+      <c r="DH32" s="12"/>
+      <c r="DI32" s="12"/>
+      <c r="DJ32" s="12"/>
+      <c r="DK32" s="12"/>
+      <c r="DL32" s="12"/>
+      <c r="DM32" s="12"/>
+      <c r="DN32" s="12"/>
+      <c r="DO32" s="12"/>
+      <c r="DP32" s="12"/>
+      <c r="DQ32" s="12"/>
+      <c r="DR32" s="12"/>
+      <c r="DS32" s="12"/>
+      <c r="DT32" s="12"/>
+      <c r="DU32" s="12"/>
+      <c r="DV32" s="12"/>
+      <c r="DW32" s="12"/>
+      <c r="DX32" s="12"/>
+      <c r="DY32" s="12"/>
+      <c r="DZ32" s="12"/>
+      <c r="EA32" s="12"/>
+      <c r="EB32" s="12"/>
+      <c r="EC32" s="12"/>
+      <c r="ED32" s="12"/>
+      <c r="EE32" s="12"/>
+      <c r="EF32" s="12"/>
+      <c r="EG32" s="12"/>
+      <c r="EH32" s="12"/>
+      <c r="EI32" s="12"/>
+      <c r="EJ32" s="12"/>
+      <c r="EK32" s="12"/>
+      <c r="EL32" s="12"/>
+      <c r="EM32" s="12"/>
+      <c r="EN32" s="12"/>
+      <c r="EO32" s="12"/>
+      <c r="EP32" s="12"/>
+      <c r="EQ32" s="12"/>
+      <c r="ER32" s="12"/>
+      <c r="ES32" s="12"/>
+      <c r="ET32" s="12"/>
+      <c r="EU32" s="12"/>
+      <c r="EV32" s="12"/>
+      <c r="EW32" s="12"/>
+      <c r="EX32" s="12"/>
+      <c r="EY32" s="12"/>
+      <c r="EZ32" s="12"/>
+      <c r="FA32" s="12"/>
+      <c r="FB32" s="12"/>
+      <c r="FC32" s="12"/>
+      <c r="FD32" s="12"/>
+      <c r="FE32" s="12"/>
+      <c r="FF32" s="12"/>
+      <c r="FG32" s="12"/>
+      <c r="FH32" s="12"/>
+      <c r="FI32" s="12"/>
+      <c r="FJ32" s="12"/>
+      <c r="FK32" s="12"/>
+      <c r="FL32" s="12"/>
+      <c r="FM32" s="12"/>
+      <c r="FN32" s="12"/>
+      <c r="FO32" s="12"/>
+      <c r="FP32" s="12"/>
+      <c r="FQ32" s="12"/>
+      <c r="FR32" s="12"/>
+      <c r="FS32" s="12"/>
+      <c r="FT32" s="12"/>
+      <c r="FU32" s="12"/>
+      <c r="FV32" s="12"/>
+      <c r="FW32" s="12"/>
+      <c r="FX32" s="12"/>
+      <c r="FY32" s="12"/>
+      <c r="FZ32" s="12"/>
+      <c r="GA32" s="12"/>
+      <c r="GB32" s="12"/>
+      <c r="GC32" s="12"/>
+      <c r="GD32" s="12"/>
+      <c r="GE32" s="12"/>
+      <c r="GF32" s="12"/>
+      <c r="GG32" s="12"/>
+      <c r="GH32" s="12"/>
+      <c r="GI32" s="12"/>
+      <c r="GJ32" s="12"/>
+      <c r="GK32" s="12"/>
+      <c r="GL32" s="12"/>
+      <c r="GM32" s="12"/>
+      <c r="GN32" s="12"/>
+      <c r="GO32" s="12"/>
+      <c r="GP32" s="12"/>
+      <c r="GQ32" s="12"/>
+      <c r="GR32" s="12"/>
+      <c r="GS32" s="12"/>
+      <c r="GT32" s="12"/>
+      <c r="GU32" s="12"/>
+      <c r="GV32" s="12"/>
+      <c r="GW32" s="12"/>
+      <c r="GX32" s="12"/>
+      <c r="GY32" s="12"/>
+      <c r="GZ32" s="12"/>
+      <c r="HA32" s="12"/>
+      <c r="HB32" s="12"/>
+      <c r="HC32" s="12"/>
+      <c r="HD32" s="12"/>
+      <c r="HE32" s="12"/>
+      <c r="HF32" s="12"/>
+      <c r="HG32" s="12"/>
+      <c r="HH32" s="12"/>
+      <c r="HI32" s="12"/>
+      <c r="HJ32" s="12"/>
+      <c r="HK32" s="12"/>
+      <c r="HL32" s="12"/>
+      <c r="HM32" s="12"/>
+      <c r="HN32" s="12"/>
+      <c r="HO32" s="12"/>
+      <c r="HP32" s="12"/>
+      <c r="HQ32" s="12"/>
+      <c r="HR32" s="12"/>
+      <c r="HS32" s="12"/>
+      <c r="HT32" s="12"/>
+      <c r="HU32" s="12"/>
+      <c r="HV32" s="12"/>
+      <c r="HW32" s="12"/>
+      <c r="HX32" s="12"/>
+      <c r="HY32" s="12"/>
+      <c r="HZ32" s="12"/>
+      <c r="IA32" s="12"/>
+      <c r="IB32" s="12"/>
+      <c r="IC32" s="12"/>
+      <c r="ID32" s="12"/>
+      <c r="IE32" s="12"/>
+      <c r="IF32" s="12"/>
+      <c r="IG32" s="12"/>
+      <c r="IH32" s="12"/>
+      <c r="II32" s="12"/>
+      <c r="IJ32" s="12"/>
+      <c r="IK32" s="12"/>
+      <c r="IL32" s="12"/>
+      <c r="IM32" s="12"/>
+      <c r="IN32" s="12"/>
+      <c r="IO32" s="12"/>
+      <c r="IP32" s="12"/>
+      <c r="IQ32" s="12"/>
+      <c r="IR32" s="12"/>
+      <c r="IS32" s="12"/>
+      <c r="IT32" s="12"/>
+      <c r="IU32" s="12"/>
+      <c r="IV32" s="12"/>
+      <c r="IW32" s="12"/>
+      <c r="IX32" s="12"/>
+      <c r="IY32" s="12"/>
+      <c r="IZ32" s="12"/>
+      <c r="JA32" s="12"/>
+      <c r="JB32" s="12"/>
+      <c r="JC32" s="12"/>
+      <c r="JD32" s="12"/>
+      <c r="JE32" s="12"/>
+      <c r="JF32" s="12"/>
+      <c r="JG32" s="12"/>
+      <c r="JH32" s="12"/>
+      <c r="JI32" s="12"/>
+      <c r="JJ32" s="12"/>
+      <c r="JK32" s="12"/>
+      <c r="JL32" s="12"/>
+      <c r="JM32" s="12"/>
+      <c r="JN32" s="12"/>
+      <c r="JO32" s="12"/>
+      <c r="JP32" s="12"/>
+      <c r="JQ32" s="12"/>
+      <c r="JR32" s="12"/>
+      <c r="JS32" s="12"/>
+      <c r="JT32" s="12"/>
+      <c r="JU32" s="12"/>
+      <c r="JV32" s="12"/>
+      <c r="JW32" s="12"/>
+      <c r="JX32" s="12"/>
+      <c r="JY32" s="12"/>
+      <c r="JZ32" s="12"/>
+      <c r="KA32" s="12"/>
+      <c r="KB32" s="12"/>
+      <c r="KC32" s="12"/>
+      <c r="KD32" s="12"/>
+      <c r="KE32" s="12"/>
+      <c r="KF32" s="12"/>
+      <c r="KG32" s="12"/>
+      <c r="KH32" s="12"/>
+      <c r="KI32" s="12"/>
+      <c r="KJ32" s="12"/>
+      <c r="KK32" s="12"/>
+      <c r="KL32" s="12"/>
+      <c r="KM32" s="12"/>
+      <c r="KN32" s="12"/>
+      <c r="KO32" s="12"/>
+      <c r="KP32" s="12"/>
+      <c r="KQ32" s="12"/>
+      <c r="KR32" s="12"/>
+      <c r="KS32" s="12"/>
+      <c r="KT32" s="12"/>
+      <c r="KU32" s="12"/>
+      <c r="KV32" s="12"/>
+      <c r="KW32" s="12"/>
+      <c r="KX32" s="12"/>
+      <c r="KY32" s="12"/>
+      <c r="KZ32" s="12"/>
+      <c r="LA32" s="12"/>
+      <c r="LB32" s="12"/>
+      <c r="LC32" s="12"/>
+      <c r="LD32" s="12"/>
+      <c r="LE32" s="12"/>
+      <c r="LF32" s="12"/>
+      <c r="LG32" s="12"/>
+      <c r="LH32" s="12"/>
+      <c r="LI32" s="12"/>
+      <c r="LJ32" s="12"/>
+      <c r="LK32" s="12"/>
+      <c r="LL32" s="12"/>
+      <c r="LM32" s="12"/>
+      <c r="LN32" s="12"/>
+      <c r="LO32" s="12"/>
+      <c r="LP32" s="12"/>
+      <c r="LQ32" s="12"/>
+      <c r="LR32" s="12"/>
+      <c r="LS32" s="12"/>
+      <c r="LT32" s="12"/>
+      <c r="LU32" s="12"/>
+      <c r="LV32" s="12"/>
+      <c r="LW32" s="12"/>
+      <c r="LX32" s="12"/>
+      <c r="LY32" s="12"/>
+      <c r="LZ32" s="12"/>
+      <c r="MA32" s="12"/>
+      <c r="MB32" s="12"/>
+      <c r="MC32" s="12"/>
+      <c r="MD32" s="12"/>
+      <c r="ME32" s="12"/>
+      <c r="MF32" s="12"/>
+      <c r="MG32" s="12"/>
+      <c r="MH32" s="12"/>
+      <c r="MI32" s="12"/>
+      <c r="MJ32" s="12"/>
+      <c r="MK32" s="12"/>
+      <c r="ML32" s="12"/>
+      <c r="MM32" s="12"/>
+      <c r="MN32" s="12"/>
+      <c r="MO32" s="12"/>
+      <c r="MP32" s="12"/>
+      <c r="MQ32" s="12"/>
+      <c r="MR32" s="12"/>
+      <c r="MS32" s="12"/>
+      <c r="MT32" s="12"/>
+      <c r="MU32" s="12"/>
+      <c r="MV32" s="12"/>
+      <c r="MW32" s="12"/>
+      <c r="MX32" s="12"/>
+      <c r="MY32" s="12"/>
+      <c r="MZ32" s="12"/>
+      <c r="NA32" s="12"/>
+      <c r="NB32" s="12"/>
+      <c r="NC32" s="12"/>
+      <c r="ND32" s="12"/>
+      <c r="NE32" s="12"/>
+      <c r="NF32" s="12"/>
+      <c r="NG32" s="12"/>
+      <c r="NH32" s="12"/>
+      <c r="NI32" s="12"/>
+      <c r="NJ32" s="12"/>
+      <c r="NK32" s="12"/>
+      <c r="NL32" s="12"/>
+      <c r="NM32" s="12"/>
+      <c r="NN32" s="12"/>
+      <c r="NO32" s="12"/>
+      <c r="NP32" s="12"/>
+      <c r="NQ32" s="12"/>
+      <c r="NR32" s="12"/>
+      <c r="NS32" s="12"/>
+      <c r="NT32" s="12"/>
+      <c r="NU32" s="12"/>
+      <c r="NV32" s="12"/>
+      <c r="NW32" s="12"/>
+      <c r="NX32" s="12"/>
+      <c r="NY32" s="12"/>
+      <c r="NZ32" s="12"/>
+      <c r="OA32" s="12"/>
+      <c r="OB32" s="12"/>
+      <c r="OC32" s="12"/>
+      <c r="OD32" s="12"/>
+      <c r="OE32" s="12"/>
+      <c r="OF32" s="12"/>
+      <c r="OG32" s="12"/>
+      <c r="OH32" s="12"/>
+      <c r="OI32" s="12"/>
+      <c r="OJ32" s="12"/>
+      <c r="OK32" s="12"/>
+      <c r="OL32" s="12"/>
+      <c r="OM32" s="12"/>
+      <c r="ON32" s="12"/>
+      <c r="OO32" s="12"/>
+      <c r="OP32" s="12"/>
+      <c r="OQ32" s="12"/>
+      <c r="OR32" s="12"/>
+      <c r="OS32" s="12"/>
+      <c r="OT32" s="12"/>
+      <c r="OU32" s="12"/>
+      <c r="OV32" s="12"/>
+      <c r="OW32" s="12"/>
+      <c r="OX32" s="12"/>
+      <c r="OY32" s="12"/>
+      <c r="OZ32" s="12"/>
+      <c r="PA32" s="12"/>
+      <c r="PB32" s="12"/>
+      <c r="PC32" s="12"/>
+      <c r="PD32" s="12"/>
+      <c r="PE32" s="12"/>
+      <c r="PF32" s="12"/>
+      <c r="PG32" s="12"/>
+      <c r="PH32" s="12"/>
+      <c r="PI32" s="12"/>
+      <c r="PJ32" s="12"/>
+      <c r="PK32" s="12"/>
+      <c r="PL32" s="12"/>
+      <c r="PM32" s="12"/>
+      <c r="PN32" s="12"/>
+      <c r="PO32" s="12"/>
+      <c r="PP32" s="12"/>
+      <c r="PQ32" s="12"/>
+      <c r="PR32" s="12"/>
+      <c r="PS32" s="12"/>
+      <c r="PT32" s="12"/>
+      <c r="PU32" s="12"/>
+      <c r="PV32" s="12"/>
+      <c r="PW32" s="12"/>
+      <c r="PX32" s="12"/>
+      <c r="PY32" s="12"/>
+      <c r="PZ32" s="12"/>
+      <c r="QA32" s="12"/>
+      <c r="QB32" s="12"/>
+      <c r="QC32" s="12"/>
+      <c r="QD32" s="12"/>
+      <c r="QE32" s="12"/>
+      <c r="QF32" s="12"/>
+      <c r="QG32" s="12"/>
+      <c r="QH32" s="12"/>
+      <c r="QI32" s="12"/>
+      <c r="QJ32" s="12"/>
+      <c r="QK32" s="12"/>
+      <c r="QL32" s="12"/>
+      <c r="QM32" s="12"/>
+      <c r="QN32" s="12"/>
+      <c r="QO32" s="12"/>
+      <c r="QP32" s="12"/>
+      <c r="QQ32" s="12"/>
+      <c r="QR32" s="12"/>
+      <c r="QS32" s="12"/>
+      <c r="QT32" s="12"/>
+      <c r="QU32" s="12"/>
+      <c r="QV32" s="12"/>
+      <c r="QW32" s="12"/>
+      <c r="QX32" s="12"/>
+      <c r="QY32" s="12"/>
+      <c r="QZ32" s="12"/>
+      <c r="RA32" s="12"/>
+      <c r="RB32" s="12"/>
+      <c r="RC32" s="12"/>
+      <c r="RD32" s="12"/>
+      <c r="RE32" s="12"/>
+      <c r="RF32" s="12"/>
+      <c r="RG32" s="12"/>
+      <c r="RH32" s="12"/>
+      <c r="RI32" s="12"/>
+      <c r="RJ32" s="12"/>
+      <c r="RK32" s="12"/>
+      <c r="RL32" s="12"/>
+      <c r="RM32" s="12"/>
+      <c r="RN32" s="12"/>
+      <c r="RO32" s="12"/>
+      <c r="RP32" s="12"/>
+      <c r="RQ32" s="12"/>
+      <c r="RR32" s="12"/>
+      <c r="RS32" s="12"/>
+      <c r="RT32" s="12"/>
+      <c r="RU32" s="12"/>
+      <c r="RV32" s="12"/>
+      <c r="RW32" s="12"/>
+      <c r="RX32" s="12"/>
+      <c r="RY32" s="12"/>
+      <c r="RZ32" s="12"/>
+      <c r="SA32" s="12"/>
+      <c r="SB32" s="12"/>
+      <c r="SC32" s="12"/>
+      <c r="SD32" s="12"/>
+      <c r="SE32" s="12"/>
+      <c r="SF32" s="12"/>
+      <c r="SG32" s="12"/>
+      <c r="SH32" s="12"/>
+      <c r="SI32" s="12"/>
+      <c r="SJ32" s="12"/>
+      <c r="SK32" s="12"/>
+      <c r="SL32" s="12"/>
+      <c r="SM32" s="12"/>
+      <c r="SN32" s="12"/>
+      <c r="SO32" s="12"/>
+      <c r="SP32" s="12"/>
+      <c r="SQ32" s="12"/>
+      <c r="SR32" s="12"/>
+      <c r="SS32" s="12"/>
+      <c r="ST32" s="12"/>
+      <c r="SU32" s="12"/>
+      <c r="SV32" s="12"/>
+      <c r="SW32" s="12"/>
+      <c r="SX32" s="12"/>
+      <c r="SY32" s="12"/>
+      <c r="SZ32" s="12"/>
+      <c r="TA32" s="12"/>
+      <c r="TB32" s="12"/>
+      <c r="TC32" s="12"/>
+      <c r="TD32" s="12"/>
+      <c r="TE32" s="12"/>
+      <c r="TF32" s="12"/>
+      <c r="TG32" s="12"/>
+      <c r="TH32" s="12"/>
+      <c r="TI32" s="12"/>
+      <c r="TJ32" s="12"/>
+      <c r="TK32" s="12"/>
+      <c r="TL32" s="12"/>
+      <c r="TM32" s="12"/>
+      <c r="TN32" s="12"/>
+      <c r="TO32" s="12"/>
+      <c r="TP32" s="12"/>
+      <c r="TQ32" s="12"/>
+      <c r="TR32" s="12"/>
+      <c r="TS32" s="12"/>
+      <c r="TT32" s="12"/>
+      <c r="TU32" s="12"/>
+      <c r="TV32" s="12"/>
+      <c r="TW32" s="12"/>
+      <c r="TX32" s="12"/>
+      <c r="TY32" s="12"/>
+      <c r="TZ32" s="12"/>
+      <c r="UA32" s="12"/>
+      <c r="UB32" s="12"/>
+      <c r="UC32" s="12"/>
+      <c r="UD32" s="12"/>
+      <c r="UE32" s="12"/>
+      <c r="UF32" s="12"/>
+      <c r="UG32" s="12"/>
+      <c r="UH32" s="12"/>
+      <c r="UI32" s="12"/>
+      <c r="UJ32" s="12"/>
+      <c r="UK32" s="12"/>
+      <c r="UL32" s="12"/>
+      <c r="UM32" s="12"/>
+      <c r="UN32" s="12"/>
+      <c r="UO32" s="12"/>
+      <c r="UP32" s="12"/>
+      <c r="UQ32" s="12"/>
+      <c r="UR32" s="12"/>
+      <c r="US32" s="12"/>
+      <c r="UT32" s="12"/>
+      <c r="UU32" s="12"/>
+      <c r="UV32" s="12"/>
+      <c r="UW32" s="12"/>
+      <c r="UX32" s="12"/>
+      <c r="UY32" s="12"/>
+      <c r="UZ32" s="12"/>
+      <c r="VA32" s="12"/>
+      <c r="VB32" s="12"/>
+      <c r="VC32" s="12"/>
+      <c r="VD32" s="12"/>
+      <c r="VE32" s="12"/>
+      <c r="VF32" s="12"/>
+      <c r="VG32" s="12"/>
+      <c r="VH32" s="12"/>
+      <c r="VI32" s="12"/>
+      <c r="VJ32" s="12"/>
+      <c r="VK32" s="12"/>
+      <c r="VL32" s="12"/>
+      <c r="VM32" s="12"/>
+      <c r="VN32" s="12"/>
+      <c r="VO32" s="12"/>
+      <c r="VP32" s="12"/>
+      <c r="VQ32" s="12"/>
+      <c r="VR32" s="12"/>
+      <c r="VS32" s="12"/>
+      <c r="VT32" s="12"/>
+      <c r="VU32" s="12"/>
+      <c r="VV32" s="12"/>
+      <c r="VW32" s="12"/>
+      <c r="VX32" s="12"/>
+      <c r="VY32" s="12"/>
+      <c r="VZ32" s="12"/>
+      <c r="WA32" s="12"/>
+      <c r="WB32" s="12"/>
+      <c r="WC32" s="12"/>
+      <c r="WD32" s="12"/>
+      <c r="WE32" s="12"/>
+      <c r="WF32" s="12"/>
+      <c r="WG32" s="12"/>
+      <c r="WH32" s="12"/>
+      <c r="WI32" s="12"/>
+      <c r="WJ32" s="12"/>
+      <c r="WK32" s="12"/>
+      <c r="WL32" s="12"/>
+      <c r="WM32" s="12"/>
+      <c r="WN32" s="12"/>
+      <c r="WO32" s="12"/>
+      <c r="WP32" s="12"/>
+      <c r="WQ32" s="12"/>
+      <c r="WR32" s="12"/>
+      <c r="WS32" s="12"/>
+      <c r="WT32" s="12"/>
+      <c r="WU32" s="12"/>
+      <c r="WV32" s="12"/>
+      <c r="WW32" s="12"/>
+      <c r="WX32" s="12"/>
+      <c r="WY32" s="12"/>
+      <c r="WZ32" s="12"/>
+      <c r="XA32" s="12"/>
+      <c r="XB32" s="12"/>
+      <c r="XC32" s="12"/>
+      <c r="XD32" s="12"/>
+      <c r="XE32" s="12"/>
+      <c r="XF32" s="12"/>
+      <c r="XG32" s="12"/>
+      <c r="XH32" s="12"/>
+      <c r="XI32" s="12"/>
+      <c r="XJ32" s="12"/>
+      <c r="XK32" s="12"/>
+      <c r="XL32" s="12"/>
+      <c r="XM32" s="12"/>
+      <c r="XN32" s="12"/>
+      <c r="XO32" s="12"/>
+      <c r="XP32" s="12"/>
+      <c r="XQ32" s="12"/>
+      <c r="XR32" s="12"/>
+      <c r="XS32" s="12"/>
+      <c r="XT32" s="12"/>
+      <c r="XU32" s="12"/>
+      <c r="XV32" s="12"/>
+      <c r="XW32" s="12"/>
+      <c r="XX32" s="12"/>
+      <c r="XY32" s="12"/>
+      <c r="XZ32" s="12"/>
+      <c r="YA32" s="12"/>
+      <c r="YB32" s="12"/>
+      <c r="YC32" s="12"/>
+      <c r="YD32" s="12"/>
+      <c r="YE32" s="12"/>
+      <c r="YF32" s="12"/>
+      <c r="YG32" s="12"/>
+      <c r="YH32" s="12"/>
+      <c r="YI32" s="12"/>
+      <c r="YJ32" s="12"/>
+      <c r="YK32" s="12"/>
+      <c r="YL32" s="12"/>
+      <c r="YM32" s="12"/>
+      <c r="YN32" s="12"/>
+      <c r="YO32" s="12"/>
+      <c r="YP32" s="12"/>
+      <c r="YQ32" s="12"/>
+      <c r="YR32" s="12"/>
+      <c r="YS32" s="12"/>
+      <c r="YT32" s="12"/>
+      <c r="YU32" s="12"/>
+      <c r="YV32" s="12"/>
+      <c r="YW32" s="12"/>
+      <c r="YX32" s="12"/>
+      <c r="YY32" s="12"/>
+      <c r="YZ32" s="12"/>
+      <c r="ZA32" s="12"/>
+      <c r="ZB32" s="12"/>
+      <c r="ZC32" s="12"/>
+      <c r="ZD32" s="12"/>
+      <c r="ZE32" s="12"/>
+      <c r="ZF32" s="12"/>
+      <c r="ZG32" s="12"/>
+      <c r="ZH32" s="12"/>
+      <c r="ZI32" s="12"/>
+      <c r="ZJ32" s="12"/>
+      <c r="ZK32" s="12"/>
+      <c r="ZL32" s="12"/>
+      <c r="ZM32" s="12"/>
+      <c r="ZN32" s="12"/>
+      <c r="ZO32" s="12"/>
+      <c r="ZP32" s="12"/>
+      <c r="ZQ32" s="12"/>
+      <c r="ZR32" s="12"/>
+      <c r="ZS32" s="12"/>
+      <c r="ZT32" s="12"/>
+      <c r="ZU32" s="12"/>
+      <c r="ZV32" s="12"/>
+      <c r="ZW32" s="12"/>
+      <c r="ZX32" s="12"/>
+      <c r="ZY32" s="12"/>
+      <c r="ZZ32" s="12"/>
+      <c r="AAA32" s="12"/>
+      <c r="AAB32" s="12"/>
+      <c r="AAC32" s="12"/>
+      <c r="AAD32" s="12"/>
+      <c r="AAE32" s="12"/>
+      <c r="AAF32" s="12"/>
+      <c r="AAG32" s="12"/>
+      <c r="AAH32" s="12"/>
+      <c r="AAI32" s="12"/>
+      <c r="AAJ32" s="12"/>
+      <c r="AAK32" s="12"/>
+      <c r="AAL32" s="12"/>
+      <c r="AAM32" s="12"/>
+      <c r="AAN32" s="12"/>
+      <c r="AAO32" s="12"/>
+      <c r="AAP32" s="12"/>
+      <c r="AAQ32" s="12"/>
+      <c r="AAR32" s="12"/>
+      <c r="AAS32" s="12"/>
+      <c r="AAT32" s="12"/>
+      <c r="AAU32" s="12"/>
+      <c r="AAV32" s="12"/>
+      <c r="AAW32" s="12"/>
+      <c r="AAX32" s="12"/>
+      <c r="AAY32" s="12"/>
+      <c r="AAZ32" s="12"/>
+      <c r="ABA32" s="12"/>
+      <c r="ABB32" s="12"/>
+      <c r="ABC32" s="12"/>
+      <c r="ABD32" s="12"/>
+      <c r="ABE32" s="12"/>
+      <c r="ABF32" s="12"/>
+      <c r="ABG32" s="12"/>
+      <c r="ABH32" s="12"/>
+      <c r="ABI32" s="12"/>
+      <c r="ABJ32" s="12"/>
+      <c r="ABK32" s="12"/>
+      <c r="ABL32" s="12"/>
+      <c r="ABM32" s="12"/>
+      <c r="ABN32" s="12"/>
+      <c r="ABO32" s="12"/>
+      <c r="ABP32" s="12"/>
+      <c r="ABQ32" s="12"/>
+      <c r="ABR32" s="12"/>
+      <c r="ABS32" s="12"/>
+      <c r="ABT32" s="12"/>
+      <c r="ABU32" s="12"/>
+      <c r="ABV32" s="12"/>
+      <c r="ABW32" s="12"/>
+      <c r="ABX32" s="12"/>
+      <c r="ABY32" s="12"/>
+      <c r="ABZ32" s="12"/>
+      <c r="ACA32" s="12"/>
+      <c r="ACB32" s="12"/>
+      <c r="ACC32" s="12"/>
+      <c r="ACD32" s="12"/>
+      <c r="ACE32" s="12"/>
+      <c r="ACF32" s="12"/>
+      <c r="ACG32" s="12"/>
+      <c r="ACH32" s="12"/>
+      <c r="ACI32" s="12"/>
+      <c r="ACJ32" s="12"/>
+      <c r="ACK32" s="12"/>
+      <c r="ACL32" s="12"/>
+      <c r="ACM32" s="12"/>
+      <c r="ACN32" s="12"/>
+      <c r="ACO32" s="12"/>
+      <c r="ACP32" s="12"/>
+      <c r="ACQ32" s="12"/>
+      <c r="ACR32" s="12"/>
+      <c r="ACS32" s="12"/>
+      <c r="ACT32" s="12"/>
+      <c r="ACU32" s="12"/>
+      <c r="ACV32" s="12"/>
+      <c r="ACW32" s="12"/>
+      <c r="ACX32" s="12"/>
+      <c r="ACY32" s="12"/>
+      <c r="ACZ32" s="12"/>
+      <c r="ADA32" s="12"/>
+      <c r="ADB32" s="12"/>
+      <c r="ADC32" s="12"/>
+      <c r="ADD32" s="12"/>
+      <c r="ADE32" s="12"/>
+      <c r="ADF32" s="12"/>
+      <c r="ADG32" s="12"/>
+      <c r="ADH32" s="12"/>
+      <c r="ADI32" s="12"/>
+      <c r="ADJ32" s="12"/>
+      <c r="ADK32" s="12"/>
+      <c r="ADL32" s="12"/>
+      <c r="ADM32" s="12"/>
+      <c r="ADN32" s="12"/>
+      <c r="ADO32" s="12"/>
+      <c r="ADP32" s="12"/>
+      <c r="ADQ32" s="12"/>
+      <c r="ADR32" s="12"/>
+      <c r="ADS32" s="12"/>
+      <c r="ADT32" s="12"/>
+      <c r="ADU32" s="12"/>
+      <c r="ADV32" s="12"/>
+      <c r="ADW32" s="12"/>
+      <c r="ADX32" s="12"/>
+      <c r="ADY32" s="12"/>
+      <c r="ADZ32" s="12"/>
+      <c r="AEA32" s="12"/>
+      <c r="AEB32" s="12"/>
+      <c r="AEC32" s="12"/>
+      <c r="AED32" s="12"/>
+      <c r="AEE32" s="12"/>
+      <c r="AEF32" s="12"/>
+      <c r="AEG32" s="12"/>
+      <c r="AEH32" s="12"/>
+      <c r="AEI32" s="12"/>
+      <c r="AEJ32" s="12"/>
+      <c r="AEK32" s="12"/>
+      <c r="AEL32" s="12"/>
+      <c r="AEM32" s="12"/>
+      <c r="AEN32" s="12"/>
+      <c r="AEO32" s="12"/>
+      <c r="AEP32" s="12"/>
+      <c r="AEQ32" s="12"/>
+      <c r="AER32" s="12"/>
+      <c r="AES32" s="12"/>
+      <c r="AET32" s="12"/>
+      <c r="AEU32" s="12"/>
+      <c r="AEV32" s="12"/>
+      <c r="AEW32" s="12"/>
+      <c r="AEX32" s="12"/>
+      <c r="AEY32" s="12"/>
+      <c r="AEZ32" s="12"/>
+      <c r="AFA32" s="12"/>
+      <c r="AFB32" s="12"/>
+      <c r="AFC32" s="12"/>
+      <c r="AFD32" s="12"/>
+      <c r="AFE32" s="12"/>
+      <c r="AFF32" s="12"/>
+      <c r="AFG32" s="12"/>
+      <c r="AFH32" s="12"/>
+      <c r="AFI32" s="12"/>
+      <c r="AFJ32" s="12"/>
+      <c r="AFK32" s="12"/>
+      <c r="AFL32" s="12"/>
+      <c r="AFM32" s="12"/>
+      <c r="AFN32" s="12"/>
+      <c r="AFO32" s="12"/>
+      <c r="AFP32" s="12"/>
+      <c r="AFQ32" s="12"/>
+      <c r="AFR32" s="12"/>
+      <c r="AFS32" s="12"/>
+      <c r="AFT32" s="12"/>
+      <c r="AFU32" s="12"/>
+      <c r="AFV32" s="12"/>
+      <c r="AFW32" s="12"/>
+      <c r="AFX32" s="12"/>
+      <c r="AFY32" s="12"/>
+      <c r="AFZ32" s="12"/>
+      <c r="AGA32" s="12"/>
+      <c r="AGB32" s="12"/>
+      <c r="AGC32" s="12"/>
+      <c r="AGD32" s="12"/>
+      <c r="AGE32" s="12"/>
+      <c r="AGF32" s="12"/>
+      <c r="AGG32" s="12"/>
+      <c r="AGH32" s="12"/>
+      <c r="AGI32" s="12"/>
+      <c r="AGJ32" s="12"/>
+      <c r="AGK32" s="12"/>
+      <c r="AGL32" s="12"/>
+      <c r="AGM32" s="12"/>
+      <c r="AGN32" s="12"/>
+      <c r="AGO32" s="12"/>
+      <c r="AGP32" s="12"/>
+      <c r="AGQ32" s="12"/>
+      <c r="AGR32" s="12"/>
+      <c r="AGS32" s="12"/>
+      <c r="AGT32" s="12"/>
+      <c r="AGU32" s="12"/>
+      <c r="AGV32" s="12"/>
+      <c r="AGW32" s="12"/>
+      <c r="AGX32" s="12"/>
+      <c r="AGY32" s="12"/>
+      <c r="AGZ32" s="12"/>
+      <c r="AHA32" s="12"/>
+      <c r="AHB32" s="12"/>
+      <c r="AHC32" s="12"/>
+      <c r="AHD32" s="12"/>
+      <c r="AHE32" s="12"/>
+      <c r="AHF32" s="12"/>
+      <c r="AHG32" s="12"/>
+      <c r="AHH32" s="12"/>
+      <c r="AHI32" s="12"/>
+      <c r="AHJ32" s="12"/>
+      <c r="AHK32" s="12"/>
+      <c r="AHL32" s="12"/>
+      <c r="AHM32" s="12"/>
+      <c r="AHN32" s="12"/>
+      <c r="AHO32" s="12"/>
+      <c r="AHP32" s="12"/>
+      <c r="AHQ32" s="12"/>
+      <c r="AHR32" s="12"/>
+      <c r="AHS32" s="12"/>
+      <c r="AHT32" s="12"/>
+      <c r="AHU32" s="12"/>
+      <c r="AHV32" s="12"/>
+      <c r="AHW32" s="12"/>
+      <c r="AHX32" s="12"/>
+      <c r="AHY32" s="12"/>
+      <c r="AHZ32" s="12"/>
+      <c r="AIA32" s="12"/>
+      <c r="AIB32" s="12"/>
+      <c r="AIC32" s="12"/>
+      <c r="AID32" s="12"/>
+      <c r="AIE32" s="12"/>
+      <c r="AIF32" s="12"/>
+      <c r="AIG32" s="12"/>
+      <c r="AIH32" s="12"/>
+      <c r="AII32" s="12"/>
+      <c r="AIJ32" s="12"/>
+      <c r="AIK32" s="12"/>
+      <c r="AIL32" s="12"/>
+      <c r="AIM32" s="12"/>
+      <c r="AIN32" s="12"/>
+      <c r="AIO32" s="12"/>
+      <c r="AIP32" s="12"/>
+      <c r="AIQ32" s="12"/>
+      <c r="AIR32" s="12"/>
+      <c r="AIS32" s="12"/>
+      <c r="AIT32" s="12"/>
+      <c r="AIU32" s="12"/>
+      <c r="AIV32" s="12"/>
+      <c r="AIW32" s="12"/>
+      <c r="AIX32" s="12"/>
+      <c r="AIY32" s="12"/>
+      <c r="AIZ32" s="12"/>
+      <c r="AJA32" s="12"/>
+      <c r="AJB32" s="12"/>
+      <c r="AJC32" s="12"/>
+      <c r="AJD32" s="12"/>
+      <c r="AJE32" s="12"/>
+      <c r="AJF32" s="12"/>
+      <c r="AJG32" s="12"/>
+      <c r="AJH32" s="12"/>
+      <c r="AJI32" s="12"/>
+      <c r="AJJ32" s="12"/>
+      <c r="AJK32" s="12"/>
+      <c r="AJL32" s="12"/>
+      <c r="AJM32" s="12"/>
+      <c r="AJN32" s="12"/>
+      <c r="AJO32" s="12"/>
+      <c r="AJP32" s="12"/>
+      <c r="AJQ32" s="12"/>
+      <c r="AJR32" s="12"/>
+      <c r="AJS32" s="12"/>
+      <c r="AJT32" s="12"/>
+      <c r="AJU32" s="12"/>
+      <c r="AJV32" s="12"/>
+      <c r="AJW32" s="12"/>
+      <c r="AJX32" s="12"/>
+      <c r="AJY32" s="12"/>
+      <c r="AJZ32" s="12"/>
+      <c r="AKA32" s="12"/>
+      <c r="AKB32" s="12"/>
+      <c r="AKC32" s="12"/>
+      <c r="AKD32" s="12"/>
+      <c r="AKE32" s="12"/>
+      <c r="AKF32" s="12"/>
+      <c r="AKG32" s="12"/>
+      <c r="AKH32" s="12"/>
+      <c r="AKI32" s="12"/>
+      <c r="AKJ32" s="12"/>
+      <c r="AKK32" s="12"/>
+      <c r="AKL32" s="12"/>
+      <c r="AKM32" s="12"/>
+      <c r="AKN32" s="12"/>
+      <c r="AKO32" s="12"/>
+      <c r="AKP32" s="12"/>
+      <c r="AKQ32" s="12"/>
+      <c r="AKR32" s="12"/>
+      <c r="AKS32" s="12"/>
+      <c r="AKT32" s="12"/>
+      <c r="AKU32" s="12"/>
+      <c r="AKV32" s="12"/>
+      <c r="AKW32" s="12"/>
+      <c r="AKX32" s="12"/>
+      <c r="AKY32" s="12"/>
+      <c r="AKZ32" s="12"/>
+      <c r="ALA32" s="12"/>
+      <c r="ALB32" s="12"/>
+      <c r="ALC32" s="12"/>
+      <c r="ALD32" s="12"/>
+      <c r="ALE32" s="12"/>
+      <c r="ALF32" s="12"/>
+      <c r="ALG32" s="12"/>
+      <c r="ALH32" s="12"/>
+      <c r="ALI32" s="12"/>
+      <c r="ALJ32" s="12"/>
+      <c r="ALK32" s="12"/>
+      <c r="ALL32" s="12"/>
+      <c r="ALM32" s="12"/>
+      <c r="ALN32" s="12"/>
+      <c r="ALO32" s="12"/>
+      <c r="ALP32" s="12"/>
+      <c r="ALQ32" s="12"/>
+      <c r="ALR32" s="12"/>
+      <c r="ALS32" s="12"/>
+      <c r="ALT32" s="12"/>
+      <c r="ALU32" s="12"/>
+      <c r="ALV32" s="12"/>
+      <c r="ALW32" s="12"/>
+      <c r="ALX32" s="12"/>
+      <c r="ALY32" s="12"/>
+      <c r="ALZ32" s="12"/>
+      <c r="AMA32" s="12"/>
+      <c r="AMB32" s="12"/>
+      <c r="AMC32" s="12"/>
+      <c r="AMD32" s="12"/>
+      <c r="AME32" s="12"/>
+      <c r="AMF32" s="12"/>
+      <c r="AMG32" s="12"/>
+      <c r="AMH32" s="12"/>
+      <c r="AMI32" s="12"/>
+      <c r="AMJ32" s="12"/>
+      <c r="AMK32" s="12"/>
+      <c r="AML32" s="12"/>
+      <c r="AMM32" s="12"/>
     </row>
-    <row r="33" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>16</v>
+    <row r="33" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>497</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>493</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>475</v>
       </c>
       <c r="G33" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K33" s="2" t="s">
-        <v>405</v>
-      </c>
+      <c r="H33" s="12"/>
+      <c r="I33" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="K33" s="15"/>
       <c r="L33" s="13" t="s">
-        <v>460</v>
-      </c>
+        <v>500</v>
+      </c>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="12"/>
+      <c r="W33" s="12"/>
+      <c r="X33" s="12"/>
+      <c r="Y33" s="12"/>
+      <c r="Z33" s="12"/>
+      <c r="AA33" s="12"/>
+      <c r="AB33" s="12"/>
+      <c r="AC33" s="12"/>
+      <c r="AD33" s="12"/>
+      <c r="AE33" s="12"/>
+      <c r="AF33" s="12"/>
+      <c r="AG33" s="12"/>
+      <c r="AH33" s="12"/>
+      <c r="AI33" s="12"/>
+      <c r="AJ33" s="12"/>
+      <c r="AK33" s="12"/>
+      <c r="AL33" s="12"/>
+      <c r="AM33" s="12"/>
+      <c r="AN33" s="12"/>
+      <c r="AO33" s="12"/>
+      <c r="AP33" s="12"/>
+      <c r="AQ33" s="12"/>
+      <c r="AR33" s="12"/>
+      <c r="AS33" s="12"/>
+      <c r="AT33" s="12"/>
+      <c r="AU33" s="12"/>
+      <c r="AV33" s="12"/>
+      <c r="AW33" s="12"/>
+      <c r="AX33" s="12"/>
+      <c r="AY33" s="12"/>
+      <c r="AZ33" s="12"/>
+      <c r="BA33" s="12"/>
+      <c r="BB33" s="12"/>
+      <c r="BC33" s="12"/>
+      <c r="BD33" s="12"/>
+      <c r="BE33" s="12"/>
+      <c r="BF33" s="12"/>
+      <c r="BG33" s="12"/>
+      <c r="BH33" s="12"/>
+      <c r="BI33" s="12"/>
+      <c r="BJ33" s="12"/>
+      <c r="BK33" s="12"/>
+      <c r="BL33" s="12"/>
+      <c r="BM33" s="12"/>
+      <c r="BN33" s="12"/>
+      <c r="BO33" s="12"/>
+      <c r="BP33" s="12"/>
+      <c r="BQ33" s="12"/>
+      <c r="BR33" s="12"/>
+      <c r="BS33" s="12"/>
+      <c r="BT33" s="12"/>
+      <c r="BU33" s="12"/>
+      <c r="BV33" s="12"/>
+      <c r="BW33" s="12"/>
+      <c r="BX33" s="12"/>
+      <c r="BY33" s="12"/>
+      <c r="BZ33" s="12"/>
+      <c r="CA33" s="12"/>
+      <c r="CB33" s="12"/>
+      <c r="CC33" s="12"/>
+      <c r="CD33" s="12"/>
+      <c r="CE33" s="12"/>
+      <c r="CF33" s="12"/>
+      <c r="CG33" s="12"/>
+      <c r="CH33" s="12"/>
+      <c r="CI33" s="12"/>
+      <c r="CJ33" s="12"/>
+      <c r="CK33" s="12"/>
+      <c r="CL33" s="12"/>
+      <c r="CM33" s="12"/>
+      <c r="CN33" s="12"/>
+      <c r="CO33" s="12"/>
+      <c r="CP33" s="12"/>
+      <c r="CQ33" s="12"/>
+      <c r="CR33" s="12"/>
+      <c r="CS33" s="12"/>
+      <c r="CT33" s="12"/>
+      <c r="CU33" s="12"/>
+      <c r="CV33" s="12"/>
+      <c r="CW33" s="12"/>
+      <c r="CX33" s="12"/>
+      <c r="CY33" s="12"/>
+      <c r="CZ33" s="12"/>
+      <c r="DA33" s="12"/>
+      <c r="DB33" s="12"/>
+      <c r="DC33" s="12"/>
+      <c r="DD33" s="12"/>
+      <c r="DE33" s="12"/>
+      <c r="DF33" s="12"/>
+      <c r="DG33" s="12"/>
+      <c r="DH33" s="12"/>
+      <c r="DI33" s="12"/>
+      <c r="DJ33" s="12"/>
+      <c r="DK33" s="12"/>
+      <c r="DL33" s="12"/>
+      <c r="DM33" s="12"/>
+      <c r="DN33" s="12"/>
+      <c r="DO33" s="12"/>
+      <c r="DP33" s="12"/>
+      <c r="DQ33" s="12"/>
+      <c r="DR33" s="12"/>
+      <c r="DS33" s="12"/>
+      <c r="DT33" s="12"/>
+      <c r="DU33" s="12"/>
+      <c r="DV33" s="12"/>
+      <c r="DW33" s="12"/>
+      <c r="DX33" s="12"/>
+      <c r="DY33" s="12"/>
+      <c r="DZ33" s="12"/>
+      <c r="EA33" s="12"/>
+      <c r="EB33" s="12"/>
+      <c r="EC33" s="12"/>
+      <c r="ED33" s="12"/>
+      <c r="EE33" s="12"/>
+      <c r="EF33" s="12"/>
+      <c r="EG33" s="12"/>
+      <c r="EH33" s="12"/>
+      <c r="EI33" s="12"/>
+      <c r="EJ33" s="12"/>
+      <c r="EK33" s="12"/>
+      <c r="EL33" s="12"/>
+      <c r="EM33" s="12"/>
+      <c r="EN33" s="12"/>
+      <c r="EO33" s="12"/>
+      <c r="EP33" s="12"/>
+      <c r="EQ33" s="12"/>
+      <c r="ER33" s="12"/>
+      <c r="ES33" s="12"/>
+      <c r="ET33" s="12"/>
+      <c r="EU33" s="12"/>
+      <c r="EV33" s="12"/>
+      <c r="EW33" s="12"/>
+      <c r="EX33" s="12"/>
+      <c r="EY33" s="12"/>
+      <c r="EZ33" s="12"/>
+      <c r="FA33" s="12"/>
+      <c r="FB33" s="12"/>
+      <c r="FC33" s="12"/>
+      <c r="FD33" s="12"/>
+      <c r="FE33" s="12"/>
+      <c r="FF33" s="12"/>
+      <c r="FG33" s="12"/>
+      <c r="FH33" s="12"/>
+      <c r="FI33" s="12"/>
+      <c r="FJ33" s="12"/>
+      <c r="FK33" s="12"/>
+      <c r="FL33" s="12"/>
+      <c r="FM33" s="12"/>
+      <c r="FN33" s="12"/>
+      <c r="FO33" s="12"/>
+      <c r="FP33" s="12"/>
+      <c r="FQ33" s="12"/>
+      <c r="FR33" s="12"/>
+      <c r="FS33" s="12"/>
+      <c r="FT33" s="12"/>
+      <c r="FU33" s="12"/>
+      <c r="FV33" s="12"/>
+      <c r="FW33" s="12"/>
+      <c r="FX33" s="12"/>
+      <c r="FY33" s="12"/>
+      <c r="FZ33" s="12"/>
+      <c r="GA33" s="12"/>
+      <c r="GB33" s="12"/>
+      <c r="GC33" s="12"/>
+      <c r="GD33" s="12"/>
+      <c r="GE33" s="12"/>
+      <c r="GF33" s="12"/>
+      <c r="GG33" s="12"/>
+      <c r="GH33" s="12"/>
+      <c r="GI33" s="12"/>
+      <c r="GJ33" s="12"/>
+      <c r="GK33" s="12"/>
+      <c r="GL33" s="12"/>
+      <c r="GM33" s="12"/>
+      <c r="GN33" s="12"/>
+      <c r="GO33" s="12"/>
+      <c r="GP33" s="12"/>
+      <c r="GQ33" s="12"/>
+      <c r="GR33" s="12"/>
+      <c r="GS33" s="12"/>
+      <c r="GT33" s="12"/>
+      <c r="GU33" s="12"/>
+      <c r="GV33" s="12"/>
+      <c r="GW33" s="12"/>
+      <c r="GX33" s="12"/>
+      <c r="GY33" s="12"/>
+      <c r="GZ33" s="12"/>
+      <c r="HA33" s="12"/>
+      <c r="HB33" s="12"/>
+      <c r="HC33" s="12"/>
+      <c r="HD33" s="12"/>
+      <c r="HE33" s="12"/>
+      <c r="HF33" s="12"/>
+      <c r="HG33" s="12"/>
+      <c r="HH33" s="12"/>
+      <c r="HI33" s="12"/>
+      <c r="HJ33" s="12"/>
+      <c r="HK33" s="12"/>
+      <c r="HL33" s="12"/>
+      <c r="HM33" s="12"/>
+      <c r="HN33" s="12"/>
+      <c r="HO33" s="12"/>
+      <c r="HP33" s="12"/>
+      <c r="HQ33" s="12"/>
+      <c r="HR33" s="12"/>
+      <c r="HS33" s="12"/>
+      <c r="HT33" s="12"/>
+      <c r="HU33" s="12"/>
+      <c r="HV33" s="12"/>
+      <c r="HW33" s="12"/>
+      <c r="HX33" s="12"/>
+      <c r="HY33" s="12"/>
+      <c r="HZ33" s="12"/>
+      <c r="IA33" s="12"/>
+      <c r="IB33" s="12"/>
+      <c r="IC33" s="12"/>
+      <c r="ID33" s="12"/>
+      <c r="IE33" s="12"/>
+      <c r="IF33" s="12"/>
+      <c r="IG33" s="12"/>
+      <c r="IH33" s="12"/>
+      <c r="II33" s="12"/>
+      <c r="IJ33" s="12"/>
+      <c r="IK33" s="12"/>
+      <c r="IL33" s="12"/>
+      <c r="IM33" s="12"/>
+      <c r="IN33" s="12"/>
+      <c r="IO33" s="12"/>
+      <c r="IP33" s="12"/>
+      <c r="IQ33" s="12"/>
+      <c r="IR33" s="12"/>
+      <c r="IS33" s="12"/>
+      <c r="IT33" s="12"/>
+      <c r="IU33" s="12"/>
+      <c r="IV33" s="12"/>
+      <c r="IW33" s="12"/>
+      <c r="IX33" s="12"/>
+      <c r="IY33" s="12"/>
+      <c r="IZ33" s="12"/>
+      <c r="JA33" s="12"/>
+      <c r="JB33" s="12"/>
+      <c r="JC33" s="12"/>
+      <c r="JD33" s="12"/>
+      <c r="JE33" s="12"/>
+      <c r="JF33" s="12"/>
+      <c r="JG33" s="12"/>
+      <c r="JH33" s="12"/>
+      <c r="JI33" s="12"/>
+      <c r="JJ33" s="12"/>
+      <c r="JK33" s="12"/>
+      <c r="JL33" s="12"/>
+      <c r="JM33" s="12"/>
+      <c r="JN33" s="12"/>
+      <c r="JO33" s="12"/>
+      <c r="JP33" s="12"/>
+      <c r="JQ33" s="12"/>
+      <c r="JR33" s="12"/>
+      <c r="JS33" s="12"/>
+      <c r="JT33" s="12"/>
+      <c r="JU33" s="12"/>
+      <c r="JV33" s="12"/>
+      <c r="JW33" s="12"/>
+      <c r="JX33" s="12"/>
+      <c r="JY33" s="12"/>
+      <c r="JZ33" s="12"/>
+      <c r="KA33" s="12"/>
+      <c r="KB33" s="12"/>
+      <c r="KC33" s="12"/>
+      <c r="KD33" s="12"/>
+      <c r="KE33" s="12"/>
+      <c r="KF33" s="12"/>
+      <c r="KG33" s="12"/>
+      <c r="KH33" s="12"/>
+      <c r="KI33" s="12"/>
+      <c r="KJ33" s="12"/>
+      <c r="KK33" s="12"/>
+      <c r="KL33" s="12"/>
+      <c r="KM33" s="12"/>
+      <c r="KN33" s="12"/>
+      <c r="KO33" s="12"/>
+      <c r="KP33" s="12"/>
+      <c r="KQ33" s="12"/>
+      <c r="KR33" s="12"/>
+      <c r="KS33" s="12"/>
+      <c r="KT33" s="12"/>
+      <c r="KU33" s="12"/>
+      <c r="KV33" s="12"/>
+      <c r="KW33" s="12"/>
+      <c r="KX33" s="12"/>
+      <c r="KY33" s="12"/>
+      <c r="KZ33" s="12"/>
+      <c r="LA33" s="12"/>
+      <c r="LB33" s="12"/>
+      <c r="LC33" s="12"/>
+      <c r="LD33" s="12"/>
+      <c r="LE33" s="12"/>
+      <c r="LF33" s="12"/>
+      <c r="LG33" s="12"/>
+      <c r="LH33" s="12"/>
+      <c r="LI33" s="12"/>
+      <c r="LJ33" s="12"/>
+      <c r="LK33" s="12"/>
+      <c r="LL33" s="12"/>
+      <c r="LM33" s="12"/>
+      <c r="LN33" s="12"/>
+      <c r="LO33" s="12"/>
+      <c r="LP33" s="12"/>
+      <c r="LQ33" s="12"/>
+      <c r="LR33" s="12"/>
+      <c r="LS33" s="12"/>
+      <c r="LT33" s="12"/>
+      <c r="LU33" s="12"/>
+      <c r="LV33" s="12"/>
+      <c r="LW33" s="12"/>
+      <c r="LX33" s="12"/>
+      <c r="LY33" s="12"/>
+      <c r="LZ33" s="12"/>
+      <c r="MA33" s="12"/>
+      <c r="MB33" s="12"/>
+      <c r="MC33" s="12"/>
+      <c r="MD33" s="12"/>
+      <c r="ME33" s="12"/>
+      <c r="MF33" s="12"/>
+      <c r="MG33" s="12"/>
+      <c r="MH33" s="12"/>
+      <c r="MI33" s="12"/>
+      <c r="MJ33" s="12"/>
+      <c r="MK33" s="12"/>
+      <c r="ML33" s="12"/>
+      <c r="MM33" s="12"/>
+      <c r="MN33" s="12"/>
+      <c r="MO33" s="12"/>
+      <c r="MP33" s="12"/>
+      <c r="MQ33" s="12"/>
+      <c r="MR33" s="12"/>
+      <c r="MS33" s="12"/>
+      <c r="MT33" s="12"/>
+      <c r="MU33" s="12"/>
+      <c r="MV33" s="12"/>
+      <c r="MW33" s="12"/>
+      <c r="MX33" s="12"/>
+      <c r="MY33" s="12"/>
+      <c r="MZ33" s="12"/>
+      <c r="NA33" s="12"/>
+      <c r="NB33" s="12"/>
+      <c r="NC33" s="12"/>
+      <c r="ND33" s="12"/>
+      <c r="NE33" s="12"/>
+      <c r="NF33" s="12"/>
+      <c r="NG33" s="12"/>
+      <c r="NH33" s="12"/>
+      <c r="NI33" s="12"/>
+      <c r="NJ33" s="12"/>
+      <c r="NK33" s="12"/>
+      <c r="NL33" s="12"/>
+      <c r="NM33" s="12"/>
+      <c r="NN33" s="12"/>
+      <c r="NO33" s="12"/>
+      <c r="NP33" s="12"/>
+      <c r="NQ33" s="12"/>
+      <c r="NR33" s="12"/>
+      <c r="NS33" s="12"/>
+      <c r="NT33" s="12"/>
+      <c r="NU33" s="12"/>
+      <c r="NV33" s="12"/>
+      <c r="NW33" s="12"/>
+      <c r="NX33" s="12"/>
+      <c r="NY33" s="12"/>
+      <c r="NZ33" s="12"/>
+      <c r="OA33" s="12"/>
+      <c r="OB33" s="12"/>
+      <c r="OC33" s="12"/>
+      <c r="OD33" s="12"/>
+      <c r="OE33" s="12"/>
+      <c r="OF33" s="12"/>
+      <c r="OG33" s="12"/>
+      <c r="OH33" s="12"/>
+      <c r="OI33" s="12"/>
+      <c r="OJ33" s="12"/>
+      <c r="OK33" s="12"/>
+      <c r="OL33" s="12"/>
+      <c r="OM33" s="12"/>
+      <c r="ON33" s="12"/>
+      <c r="OO33" s="12"/>
+      <c r="OP33" s="12"/>
+      <c r="OQ33" s="12"/>
+      <c r="OR33" s="12"/>
+      <c r="OS33" s="12"/>
+      <c r="OT33" s="12"/>
+      <c r="OU33" s="12"/>
+      <c r="OV33" s="12"/>
+      <c r="OW33" s="12"/>
+      <c r="OX33" s="12"/>
+      <c r="OY33" s="12"/>
+      <c r="OZ33" s="12"/>
+      <c r="PA33" s="12"/>
+      <c r="PB33" s="12"/>
+      <c r="PC33" s="12"/>
+      <c r="PD33" s="12"/>
+      <c r="PE33" s="12"/>
+      <c r="PF33" s="12"/>
+      <c r="PG33" s="12"/>
+      <c r="PH33" s="12"/>
+      <c r="PI33" s="12"/>
+      <c r="PJ33" s="12"/>
+      <c r="PK33" s="12"/>
+      <c r="PL33" s="12"/>
+      <c r="PM33" s="12"/>
+      <c r="PN33" s="12"/>
+      <c r="PO33" s="12"/>
+      <c r="PP33" s="12"/>
+      <c r="PQ33" s="12"/>
+      <c r="PR33" s="12"/>
+      <c r="PS33" s="12"/>
+      <c r="PT33" s="12"/>
+      <c r="PU33" s="12"/>
+      <c r="PV33" s="12"/>
+      <c r="PW33" s="12"/>
+      <c r="PX33" s="12"/>
+      <c r="PY33" s="12"/>
+      <c r="PZ33" s="12"/>
+      <c r="QA33" s="12"/>
+      <c r="QB33" s="12"/>
+      <c r="QC33" s="12"/>
+      <c r="QD33" s="12"/>
+      <c r="QE33" s="12"/>
+      <c r="QF33" s="12"/>
+      <c r="QG33" s="12"/>
+      <c r="QH33" s="12"/>
+      <c r="QI33" s="12"/>
+      <c r="QJ33" s="12"/>
+      <c r="QK33" s="12"/>
+      <c r="QL33" s="12"/>
+      <c r="QM33" s="12"/>
+      <c r="QN33" s="12"/>
+      <c r="QO33" s="12"/>
+      <c r="QP33" s="12"/>
+      <c r="QQ33" s="12"/>
+      <c r="QR33" s="12"/>
+      <c r="QS33" s="12"/>
+      <c r="QT33" s="12"/>
+      <c r="QU33" s="12"/>
+      <c r="QV33" s="12"/>
+      <c r="QW33" s="12"/>
+      <c r="QX33" s="12"/>
+      <c r="QY33" s="12"/>
+      <c r="QZ33" s="12"/>
+      <c r="RA33" s="12"/>
+      <c r="RB33" s="12"/>
+      <c r="RC33" s="12"/>
+      <c r="RD33" s="12"/>
+      <c r="RE33" s="12"/>
+      <c r="RF33" s="12"/>
+      <c r="RG33" s="12"/>
+      <c r="RH33" s="12"/>
+      <c r="RI33" s="12"/>
+      <c r="RJ33" s="12"/>
+      <c r="RK33" s="12"/>
+      <c r="RL33" s="12"/>
+      <c r="RM33" s="12"/>
+      <c r="RN33" s="12"/>
+      <c r="RO33" s="12"/>
+      <c r="RP33" s="12"/>
+      <c r="RQ33" s="12"/>
+      <c r="RR33" s="12"/>
+      <c r="RS33" s="12"/>
+      <c r="RT33" s="12"/>
+      <c r="RU33" s="12"/>
+      <c r="RV33" s="12"/>
+      <c r="RW33" s="12"/>
+      <c r="RX33" s="12"/>
+      <c r="RY33" s="12"/>
+      <c r="RZ33" s="12"/>
+      <c r="SA33" s="12"/>
+      <c r="SB33" s="12"/>
+      <c r="SC33" s="12"/>
+      <c r="SD33" s="12"/>
+      <c r="SE33" s="12"/>
+      <c r="SF33" s="12"/>
+      <c r="SG33" s="12"/>
+      <c r="SH33" s="12"/>
+      <c r="SI33" s="12"/>
+      <c r="SJ33" s="12"/>
+      <c r="SK33" s="12"/>
+      <c r="SL33" s="12"/>
+      <c r="SM33" s="12"/>
+      <c r="SN33" s="12"/>
+      <c r="SO33" s="12"/>
+      <c r="SP33" s="12"/>
+      <c r="SQ33" s="12"/>
+      <c r="SR33" s="12"/>
+      <c r="SS33" s="12"/>
+      <c r="ST33" s="12"/>
+      <c r="SU33" s="12"/>
+      <c r="SV33" s="12"/>
+      <c r="SW33" s="12"/>
+      <c r="SX33" s="12"/>
+      <c r="SY33" s="12"/>
+      <c r="SZ33" s="12"/>
+      <c r="TA33" s="12"/>
+      <c r="TB33" s="12"/>
+      <c r="TC33" s="12"/>
+      <c r="TD33" s="12"/>
+      <c r="TE33" s="12"/>
+      <c r="TF33" s="12"/>
+      <c r="TG33" s="12"/>
+      <c r="TH33" s="12"/>
+      <c r="TI33" s="12"/>
+      <c r="TJ33" s="12"/>
+      <c r="TK33" s="12"/>
+      <c r="TL33" s="12"/>
+      <c r="TM33" s="12"/>
+      <c r="TN33" s="12"/>
+      <c r="TO33" s="12"/>
+      <c r="TP33" s="12"/>
+      <c r="TQ33" s="12"/>
+      <c r="TR33" s="12"/>
+      <c r="TS33" s="12"/>
+      <c r="TT33" s="12"/>
+      <c r="TU33" s="12"/>
+      <c r="TV33" s="12"/>
+      <c r="TW33" s="12"/>
+      <c r="TX33" s="12"/>
+      <c r="TY33" s="12"/>
+      <c r="TZ33" s="12"/>
+      <c r="UA33" s="12"/>
+      <c r="UB33" s="12"/>
+      <c r="UC33" s="12"/>
+      <c r="UD33" s="12"/>
+      <c r="UE33" s="12"/>
+      <c r="UF33" s="12"/>
+      <c r="UG33" s="12"/>
+      <c r="UH33" s="12"/>
+      <c r="UI33" s="12"/>
+      <c r="UJ33" s="12"/>
+      <c r="UK33" s="12"/>
+      <c r="UL33" s="12"/>
+      <c r="UM33" s="12"/>
+      <c r="UN33" s="12"/>
+      <c r="UO33" s="12"/>
+      <c r="UP33" s="12"/>
+      <c r="UQ33" s="12"/>
+      <c r="UR33" s="12"/>
+      <c r="US33" s="12"/>
+      <c r="UT33" s="12"/>
+      <c r="UU33" s="12"/>
+      <c r="UV33" s="12"/>
+      <c r="UW33" s="12"/>
+      <c r="UX33" s="12"/>
+      <c r="UY33" s="12"/>
+      <c r="UZ33" s="12"/>
+      <c r="VA33" s="12"/>
+      <c r="VB33" s="12"/>
+      <c r="VC33" s="12"/>
+      <c r="VD33" s="12"/>
+      <c r="VE33" s="12"/>
+      <c r="VF33" s="12"/>
+      <c r="VG33" s="12"/>
+      <c r="VH33" s="12"/>
+      <c r="VI33" s="12"/>
+      <c r="VJ33" s="12"/>
+      <c r="VK33" s="12"/>
+      <c r="VL33" s="12"/>
+      <c r="VM33" s="12"/>
+      <c r="VN33" s="12"/>
+      <c r="VO33" s="12"/>
+      <c r="VP33" s="12"/>
+      <c r="VQ33" s="12"/>
+      <c r="VR33" s="12"/>
+      <c r="VS33" s="12"/>
+      <c r="VT33" s="12"/>
+      <c r="VU33" s="12"/>
+      <c r="VV33" s="12"/>
+      <c r="VW33" s="12"/>
+      <c r="VX33" s="12"/>
+      <c r="VY33" s="12"/>
+      <c r="VZ33" s="12"/>
+      <c r="WA33" s="12"/>
+      <c r="WB33" s="12"/>
+      <c r="WC33" s="12"/>
+      <c r="WD33" s="12"/>
+      <c r="WE33" s="12"/>
+      <c r="WF33" s="12"/>
+      <c r="WG33" s="12"/>
+      <c r="WH33" s="12"/>
+      <c r="WI33" s="12"/>
+      <c r="WJ33" s="12"/>
+      <c r="WK33" s="12"/>
+      <c r="WL33" s="12"/>
+      <c r="WM33" s="12"/>
+      <c r="WN33" s="12"/>
+      <c r="WO33" s="12"/>
+      <c r="WP33" s="12"/>
+      <c r="WQ33" s="12"/>
+      <c r="WR33" s="12"/>
+      <c r="WS33" s="12"/>
+      <c r="WT33" s="12"/>
+      <c r="WU33" s="12"/>
+      <c r="WV33" s="12"/>
+      <c r="WW33" s="12"/>
+      <c r="WX33" s="12"/>
+      <c r="WY33" s="12"/>
+      <c r="WZ33" s="12"/>
+      <c r="XA33" s="12"/>
+      <c r="XB33" s="12"/>
+      <c r="XC33" s="12"/>
+      <c r="XD33" s="12"/>
+      <c r="XE33" s="12"/>
+      <c r="XF33" s="12"/>
+      <c r="XG33" s="12"/>
+      <c r="XH33" s="12"/>
+      <c r="XI33" s="12"/>
+      <c r="XJ33" s="12"/>
+      <c r="XK33" s="12"/>
+      <c r="XL33" s="12"/>
+      <c r="XM33" s="12"/>
+      <c r="XN33" s="12"/>
+      <c r="XO33" s="12"/>
+      <c r="XP33" s="12"/>
+      <c r="XQ33" s="12"/>
+      <c r="XR33" s="12"/>
+      <c r="XS33" s="12"/>
+      <c r="XT33" s="12"/>
+      <c r="XU33" s="12"/>
+      <c r="XV33" s="12"/>
+      <c r="XW33" s="12"/>
+      <c r="XX33" s="12"/>
+      <c r="XY33" s="12"/>
+      <c r="XZ33" s="12"/>
+      <c r="YA33" s="12"/>
+      <c r="YB33" s="12"/>
+      <c r="YC33" s="12"/>
+      <c r="YD33" s="12"/>
+      <c r="YE33" s="12"/>
+      <c r="YF33" s="12"/>
+      <c r="YG33" s="12"/>
+      <c r="YH33" s="12"/>
+      <c r="YI33" s="12"/>
+      <c r="YJ33" s="12"/>
+      <c r="YK33" s="12"/>
+      <c r="YL33" s="12"/>
+      <c r="YM33" s="12"/>
+      <c r="YN33" s="12"/>
+      <c r="YO33" s="12"/>
+      <c r="YP33" s="12"/>
+      <c r="YQ33" s="12"/>
+      <c r="YR33" s="12"/>
+      <c r="YS33" s="12"/>
+      <c r="YT33" s="12"/>
+      <c r="YU33" s="12"/>
+      <c r="YV33" s="12"/>
+      <c r="YW33" s="12"/>
+      <c r="YX33" s="12"/>
+      <c r="YY33" s="12"/>
+      <c r="YZ33" s="12"/>
+      <c r="ZA33" s="12"/>
+      <c r="ZB33" s="12"/>
+      <c r="ZC33" s="12"/>
+      <c r="ZD33" s="12"/>
+      <c r="ZE33" s="12"/>
+      <c r="ZF33" s="12"/>
+      <c r="ZG33" s="12"/>
+      <c r="ZH33" s="12"/>
+      <c r="ZI33" s="12"/>
+      <c r="ZJ33" s="12"/>
+      <c r="ZK33" s="12"/>
+      <c r="ZL33" s="12"/>
+      <c r="ZM33" s="12"/>
+      <c r="ZN33" s="12"/>
+      <c r="ZO33" s="12"/>
+      <c r="ZP33" s="12"/>
+      <c r="ZQ33" s="12"/>
+      <c r="ZR33" s="12"/>
+      <c r="ZS33" s="12"/>
+      <c r="ZT33" s="12"/>
+      <c r="ZU33" s="12"/>
+      <c r="ZV33" s="12"/>
+      <c r="ZW33" s="12"/>
+      <c r="ZX33" s="12"/>
+      <c r="ZY33" s="12"/>
+      <c r="ZZ33" s="12"/>
+      <c r="AAA33" s="12"/>
+      <c r="AAB33" s="12"/>
+      <c r="AAC33" s="12"/>
+      <c r="AAD33" s="12"/>
+      <c r="AAE33" s="12"/>
+      <c r="AAF33" s="12"/>
+      <c r="AAG33" s="12"/>
+      <c r="AAH33" s="12"/>
+      <c r="AAI33" s="12"/>
+      <c r="AAJ33" s="12"/>
+      <c r="AAK33" s="12"/>
+      <c r="AAL33" s="12"/>
+      <c r="AAM33" s="12"/>
+      <c r="AAN33" s="12"/>
+      <c r="AAO33" s="12"/>
+      <c r="AAP33" s="12"/>
+      <c r="AAQ33" s="12"/>
+      <c r="AAR33" s="12"/>
+      <c r="AAS33" s="12"/>
+      <c r="AAT33" s="12"/>
+      <c r="AAU33" s="12"/>
+      <c r="AAV33" s="12"/>
+      <c r="AAW33" s="12"/>
+      <c r="AAX33" s="12"/>
+      <c r="AAY33" s="12"/>
+      <c r="AAZ33" s="12"/>
+      <c r="ABA33" s="12"/>
+      <c r="ABB33" s="12"/>
+      <c r="ABC33" s="12"/>
+      <c r="ABD33" s="12"/>
+      <c r="ABE33" s="12"/>
+      <c r="ABF33" s="12"/>
+      <c r="ABG33" s="12"/>
+      <c r="ABH33" s="12"/>
+      <c r="ABI33" s="12"/>
+      <c r="ABJ33" s="12"/>
+      <c r="ABK33" s="12"/>
+      <c r="ABL33" s="12"/>
+      <c r="ABM33" s="12"/>
+      <c r="ABN33" s="12"/>
+      <c r="ABO33" s="12"/>
+      <c r="ABP33" s="12"/>
+      <c r="ABQ33" s="12"/>
+      <c r="ABR33" s="12"/>
+      <c r="ABS33" s="12"/>
+      <c r="ABT33" s="12"/>
+      <c r="ABU33" s="12"/>
+      <c r="ABV33" s="12"/>
+      <c r="ABW33" s="12"/>
+      <c r="ABX33" s="12"/>
+      <c r="ABY33" s="12"/>
+      <c r="ABZ33" s="12"/>
+      <c r="ACA33" s="12"/>
+      <c r="ACB33" s="12"/>
+      <c r="ACC33" s="12"/>
+      <c r="ACD33" s="12"/>
+      <c r="ACE33" s="12"/>
+      <c r="ACF33" s="12"/>
+      <c r="ACG33" s="12"/>
+      <c r="ACH33" s="12"/>
+      <c r="ACI33" s="12"/>
+      <c r="ACJ33" s="12"/>
+      <c r="ACK33" s="12"/>
+      <c r="ACL33" s="12"/>
+      <c r="ACM33" s="12"/>
+      <c r="ACN33" s="12"/>
+      <c r="ACO33" s="12"/>
+      <c r="ACP33" s="12"/>
+      <c r="ACQ33" s="12"/>
+      <c r="ACR33" s="12"/>
+      <c r="ACS33" s="12"/>
+      <c r="ACT33" s="12"/>
+      <c r="ACU33" s="12"/>
+      <c r="ACV33" s="12"/>
+      <c r="ACW33" s="12"/>
+      <c r="ACX33" s="12"/>
+      <c r="ACY33" s="12"/>
+      <c r="ACZ33" s="12"/>
+      <c r="ADA33" s="12"/>
+      <c r="ADB33" s="12"/>
+      <c r="ADC33" s="12"/>
+      <c r="ADD33" s="12"/>
+      <c r="ADE33" s="12"/>
+      <c r="ADF33" s="12"/>
+      <c r="ADG33" s="12"/>
+      <c r="ADH33" s="12"/>
+      <c r="ADI33" s="12"/>
+      <c r="ADJ33" s="12"/>
+      <c r="ADK33" s="12"/>
+      <c r="ADL33" s="12"/>
+      <c r="ADM33" s="12"/>
+      <c r="ADN33" s="12"/>
+      <c r="ADO33" s="12"/>
+      <c r="ADP33" s="12"/>
+      <c r="ADQ33" s="12"/>
+      <c r="ADR33" s="12"/>
+      <c r="ADS33" s="12"/>
+      <c r="ADT33" s="12"/>
+      <c r="ADU33" s="12"/>
+      <c r="ADV33" s="12"/>
+      <c r="ADW33" s="12"/>
+      <c r="ADX33" s="12"/>
+      <c r="ADY33" s="12"/>
+      <c r="ADZ33" s="12"/>
+      <c r="AEA33" s="12"/>
+      <c r="AEB33" s="12"/>
+      <c r="AEC33" s="12"/>
+      <c r="AED33" s="12"/>
+      <c r="AEE33" s="12"/>
+      <c r="AEF33" s="12"/>
+      <c r="AEG33" s="12"/>
+      <c r="AEH33" s="12"/>
+      <c r="AEI33" s="12"/>
+      <c r="AEJ33" s="12"/>
+      <c r="AEK33" s="12"/>
+      <c r="AEL33" s="12"/>
+      <c r="AEM33" s="12"/>
+      <c r="AEN33" s="12"/>
+      <c r="AEO33" s="12"/>
+      <c r="AEP33" s="12"/>
+      <c r="AEQ33" s="12"/>
+      <c r="AER33" s="12"/>
+      <c r="AES33" s="12"/>
+      <c r="AET33" s="12"/>
+      <c r="AEU33" s="12"/>
+      <c r="AEV33" s="12"/>
+      <c r="AEW33" s="12"/>
+      <c r="AEX33" s="12"/>
+      <c r="AEY33" s="12"/>
+      <c r="AEZ33" s="12"/>
+      <c r="AFA33" s="12"/>
+      <c r="AFB33" s="12"/>
+      <c r="AFC33" s="12"/>
+      <c r="AFD33" s="12"/>
+      <c r="AFE33" s="12"/>
+      <c r="AFF33" s="12"/>
+      <c r="AFG33" s="12"/>
+      <c r="AFH33" s="12"/>
+      <c r="AFI33" s="12"/>
+      <c r="AFJ33" s="12"/>
+      <c r="AFK33" s="12"/>
+      <c r="AFL33" s="12"/>
+      <c r="AFM33" s="12"/>
+      <c r="AFN33" s="12"/>
+      <c r="AFO33" s="12"/>
+      <c r="AFP33" s="12"/>
+      <c r="AFQ33" s="12"/>
+      <c r="AFR33" s="12"/>
+      <c r="AFS33" s="12"/>
+      <c r="AFT33" s="12"/>
+      <c r="AFU33" s="12"/>
+      <c r="AFV33" s="12"/>
+      <c r="AFW33" s="12"/>
+      <c r="AFX33" s="12"/>
+      <c r="AFY33" s="12"/>
+      <c r="AFZ33" s="12"/>
+      <c r="AGA33" s="12"/>
+      <c r="AGB33" s="12"/>
+      <c r="AGC33" s="12"/>
+      <c r="AGD33" s="12"/>
+      <c r="AGE33" s="12"/>
+      <c r="AGF33" s="12"/>
+      <c r="AGG33" s="12"/>
+      <c r="AGH33" s="12"/>
+      <c r="AGI33" s="12"/>
+      <c r="AGJ33" s="12"/>
+      <c r="AGK33" s="12"/>
+      <c r="AGL33" s="12"/>
+      <c r="AGM33" s="12"/>
+      <c r="AGN33" s="12"/>
+      <c r="AGO33" s="12"/>
+      <c r="AGP33" s="12"/>
+      <c r="AGQ33" s="12"/>
+      <c r="AGR33" s="12"/>
+      <c r="AGS33" s="12"/>
+      <c r="AGT33" s="12"/>
+      <c r="AGU33" s="12"/>
+      <c r="AGV33" s="12"/>
+      <c r="AGW33" s="12"/>
+      <c r="AGX33" s="12"/>
+      <c r="AGY33" s="12"/>
+      <c r="AGZ33" s="12"/>
+      <c r="AHA33" s="12"/>
+      <c r="AHB33" s="12"/>
+      <c r="AHC33" s="12"/>
+      <c r="AHD33" s="12"/>
+      <c r="AHE33" s="12"/>
+      <c r="AHF33" s="12"/>
+      <c r="AHG33" s="12"/>
+      <c r="AHH33" s="12"/>
+      <c r="AHI33" s="12"/>
+      <c r="AHJ33" s="12"/>
+      <c r="AHK33" s="12"/>
+      <c r="AHL33" s="12"/>
+      <c r="AHM33" s="12"/>
+      <c r="AHN33" s="12"/>
+      <c r="AHO33" s="12"/>
+      <c r="AHP33" s="12"/>
+      <c r="AHQ33" s="12"/>
+      <c r="AHR33" s="12"/>
+      <c r="AHS33" s="12"/>
+      <c r="AHT33" s="12"/>
+      <c r="AHU33" s="12"/>
+      <c r="AHV33" s="12"/>
+      <c r="AHW33" s="12"/>
+      <c r="AHX33" s="12"/>
+      <c r="AHY33" s="12"/>
+      <c r="AHZ33" s="12"/>
+      <c r="AIA33" s="12"/>
+      <c r="AIB33" s="12"/>
+      <c r="AIC33" s="12"/>
+      <c r="AID33" s="12"/>
+      <c r="AIE33" s="12"/>
+      <c r="AIF33" s="12"/>
+      <c r="AIG33" s="12"/>
+      <c r="AIH33" s="12"/>
+      <c r="AII33" s="12"/>
+      <c r="AIJ33" s="12"/>
+      <c r="AIK33" s="12"/>
+      <c r="AIL33" s="12"/>
+      <c r="AIM33" s="12"/>
+      <c r="AIN33" s="12"/>
+      <c r="AIO33" s="12"/>
+      <c r="AIP33" s="12"/>
+      <c r="AIQ33" s="12"/>
+      <c r="AIR33" s="12"/>
+      <c r="AIS33" s="12"/>
+      <c r="AIT33" s="12"/>
+      <c r="AIU33" s="12"/>
+      <c r="AIV33" s="12"/>
+      <c r="AIW33" s="12"/>
+      <c r="AIX33" s="12"/>
+      <c r="AIY33" s="12"/>
+      <c r="AIZ33" s="12"/>
+      <c r="AJA33" s="12"/>
+      <c r="AJB33" s="12"/>
+      <c r="AJC33" s="12"/>
+      <c r="AJD33" s="12"/>
+      <c r="AJE33" s="12"/>
+      <c r="AJF33" s="12"/>
+      <c r="AJG33" s="12"/>
+      <c r="AJH33" s="12"/>
+      <c r="AJI33" s="12"/>
+      <c r="AJJ33" s="12"/>
+      <c r="AJK33" s="12"/>
+      <c r="AJL33" s="12"/>
+      <c r="AJM33" s="12"/>
+      <c r="AJN33" s="12"/>
+      <c r="AJO33" s="12"/>
+      <c r="AJP33" s="12"/>
+      <c r="AJQ33" s="12"/>
+      <c r="AJR33" s="12"/>
+      <c r="AJS33" s="12"/>
+      <c r="AJT33" s="12"/>
+      <c r="AJU33" s="12"/>
+      <c r="AJV33" s="12"/>
+      <c r="AJW33" s="12"/>
+      <c r="AJX33" s="12"/>
+      <c r="AJY33" s="12"/>
+      <c r="AJZ33" s="12"/>
+      <c r="AKA33" s="12"/>
+      <c r="AKB33" s="12"/>
+      <c r="AKC33" s="12"/>
+      <c r="AKD33" s="12"/>
+      <c r="AKE33" s="12"/>
+      <c r="AKF33" s="12"/>
+      <c r="AKG33" s="12"/>
+      <c r="AKH33" s="12"/>
+      <c r="AKI33" s="12"/>
+      <c r="AKJ33" s="12"/>
+      <c r="AKK33" s="12"/>
+      <c r="AKL33" s="12"/>
+      <c r="AKM33" s="12"/>
+      <c r="AKN33" s="12"/>
+      <c r="AKO33" s="12"/>
+      <c r="AKP33" s="12"/>
+      <c r="AKQ33" s="12"/>
+      <c r="AKR33" s="12"/>
+      <c r="AKS33" s="12"/>
+      <c r="AKT33" s="12"/>
+      <c r="AKU33" s="12"/>
+      <c r="AKV33" s="12"/>
+      <c r="AKW33" s="12"/>
+      <c r="AKX33" s="12"/>
+      <c r="AKY33" s="12"/>
+      <c r="AKZ33" s="12"/>
+      <c r="ALA33" s="12"/>
+      <c r="ALB33" s="12"/>
+      <c r="ALC33" s="12"/>
+      <c r="ALD33" s="12"/>
+      <c r="ALE33" s="12"/>
+      <c r="ALF33" s="12"/>
+      <c r="ALG33" s="12"/>
+      <c r="ALH33" s="12"/>
+      <c r="ALI33" s="12"/>
+      <c r="ALJ33" s="12"/>
+      <c r="ALK33" s="12"/>
+      <c r="ALL33" s="12"/>
+      <c r="ALM33" s="12"/>
+      <c r="ALN33" s="12"/>
+      <c r="ALO33" s="12"/>
+      <c r="ALP33" s="12"/>
+      <c r="ALQ33" s="12"/>
+      <c r="ALR33" s="12"/>
+      <c r="ALS33" s="12"/>
+      <c r="ALT33" s="12"/>
+      <c r="ALU33" s="12"/>
+      <c r="ALV33" s="12"/>
+      <c r="ALW33" s="12"/>
+      <c r="ALX33" s="12"/>
+      <c r="ALY33" s="12"/>
+      <c r="ALZ33" s="12"/>
+      <c r="AMA33" s="12"/>
+      <c r="AMB33" s="12"/>
+      <c r="AMC33" s="12"/>
+      <c r="AMD33" s="12"/>
+      <c r="AME33" s="12"/>
+      <c r="AMF33" s="12"/>
+      <c r="AMG33" s="12"/>
+      <c r="AMH33" s="12"/>
+      <c r="AMI33" s="12"/>
+      <c r="AMJ33" s="12"/>
+      <c r="AMK33" s="12"/>
+      <c r="AML33" s="12"/>
+      <c r="AMM33" s="12"/>
     </row>
-    <row r="34" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>16</v>
@@ -6639,28 +8763,31 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K34" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="L34" s="13" t="s">
-        <v>461</v>
+      <c r="I34" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>420</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>16</v>
@@ -6670,24 +8797,27 @@
         <v>0</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>421</v>
+        <v>405</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>460</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>16</v>
@@ -6697,27 +8827,27 @@
         <v>0</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="L36" s="13" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="285" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>16</v>
@@ -6727,30 +8857,24 @@
         <v>0</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="L37" s="13" t="s">
-        <v>463</v>
+        <v>137</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1027" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>16</v>
@@ -6759,64 +8883,61 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="I38" s="8" t="s">
-        <v>103</v>
+      <c r="K38" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="L38" s="13" t="s">
-        <v>451</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>423</v>
+        <v>462</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1027" ht="285" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>347</v>
+        <v>147</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G39" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>153</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>158</v>
+        <v>406</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1027" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>16</v>
@@ -6825,24 +8946,32 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
+      <c r="I40" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="L40" s="13" t="s">
-        <v>465</v>
+        <v>451</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>423</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E41" s="9"/>
+        <v>347</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="F41" s="1" t="s">
         <v>16</v>
       </c>
@@ -6853,31 +8982,28 @@
       <c r="H41" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I41" s="8" t="s">
-        <v>162</v>
+      <c r="K41" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="L41" s="13" t="s">
-        <v>466</v>
-      </c>
-      <c r="M41" s="12" t="s">
-        <v>469</v>
+        <v>464</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>424</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1027" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>38</v>
+        <v>156</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>16</v>
@@ -6886,48 +9012,60 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="M42" s="1" t="s">
-        <v>425</v>
+      <c r="L42" s="13" t="s">
+        <v>465</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1027" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>168</v>
+        <v>38</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>169</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="E43" s="9"/>
       <c r="F43" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G43" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>171</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I43" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="L43" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="M43" s="12" t="s">
+        <v>469</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>168</v>
+        <v>38</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E44" s="9"/>
+        <v>165</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>165</v>
+      </c>
       <c r="F44" s="1" t="s">
         <v>16</v>
       </c>
@@ -6935,241 +9073,246 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K44" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="L44" s="13" t="s">
-        <v>467</v>
-      </c>
       <c r="M44" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>168</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G45" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" s="9"/>
+      <c r="F46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="48" spans="1:1027" ht="105" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G46" s="7" t="b">
+      <c r="G48" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I46" s="8" t="s">
+      <c r="I48" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="J46" s="8" t="s">
+      <c r="J48" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="L46" s="13" t="s">
+      <c r="L48" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="M48" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="49" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="G47" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E48" s="9"/>
-      <c r="F48" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G48" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="I48" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="G49" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
+      <c r="I49" s="8" t="s">
+        <v>388</v>
+      </c>
     </row>
-    <row r="50" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>54</v>
+        <v>168</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>182</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="E50" s="9"/>
       <c r="F50" s="1" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="G50" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>363</v>
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="I50" s="8" t="s">
+        <v>190</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>196</v>
+    <row r="51" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E51" s="9"/>
+        <v>178</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>178</v>
+      </c>
       <c r="F51" s="1" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="G51" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>200</v>
+    <row r="52" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>202</v>
+        <v>54</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E52" s="9"/>
+        <v>182</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="F52" s="1" t="s">
         <v>153</v>
       </c>
       <c r="G52" s="7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="E53" s="9"/>
       <c r="F53" s="1" t="s">
@@ -7182,16 +9325,16 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>106</v>
+        <v>202</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="1" t="s">
@@ -7204,16 +9347,16 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E55" s="9"/>
       <c r="F55" s="1" t="s">
@@ -7226,16 +9369,16 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>217</v>
+        <v>106</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E56" s="9"/>
       <c r="F56" s="1" t="s">
@@ -7248,17 +9391,18 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>222</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="E57" s="9"/>
       <c r="F57" s="1" t="s">
         <v>153</v>
       </c>
@@ -7269,16 +9413,16 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="E58" s="9"/>
       <c r="F58" s="1" t="s">
@@ -7291,18 +9435,17 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E59" s="9"/>
+        <v>222</v>
+      </c>
       <c r="F59" s="1" t="s">
         <v>153</v>
       </c>
@@ -7313,16 +9456,16 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>95</v>
+        <v>225</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="1" t="s">
@@ -7334,17 +9477,17 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
-        <v>234</v>
+      <c r="A61" s="10" t="s">
+        <v>227</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="E61" s="9"/>
       <c r="F61" s="1" t="s">
@@ -7356,17 +9499,17 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
-        <v>238</v>
+      <c r="A62" s="10" t="s">
+        <v>231</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>240</v>
+        <v>95</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E62" s="9"/>
       <c r="F62" s="1" t="s">
@@ -7379,16 +9522,16 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E63" s="9"/>
       <c r="F63" s="1" t="s">
@@ -7401,16 +9544,16 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="E64" s="9"/>
       <c r="F64" s="1" t="s">
@@ -7423,16 +9566,16 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E65" s="9"/>
       <c r="F65" s="1" t="s">
@@ -7445,16 +9588,16 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>123</v>
+        <v>248</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="E66" s="9"/>
       <c r="F66" s="1" t="s">
@@ -7467,16 +9610,16 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E67" s="9"/>
       <c r="F67" s="1" t="s">
@@ -7489,16 +9632,16 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>263</v>
+        <v>123</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="E68" s="9"/>
       <c r="F68" s="1" t="s">
@@ -7511,16 +9654,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="E69" s="9"/>
       <c r="F69" s="1" t="s">
@@ -7533,16 +9676,16 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="E70" s="9"/>
       <c r="F70" s="1" t="s">
@@ -7553,18 +9696,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="E71" s="9"/>
       <c r="F71" s="1" t="s">
@@ -7577,16 +9720,16 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E72" s="9"/>
       <c r="F72" s="1" t="s">
@@ -7597,18 +9740,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>58</v>
+        <v>275</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="E73" s="9"/>
       <c r="F73" s="1" t="s">
@@ -7621,16 +9764,16 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E74" s="9"/>
       <c r="F74" s="1" t="s">
@@ -7643,16 +9786,16 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>290</v>
+        <v>58</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="E75" s="9"/>
       <c r="F75" s="1" t="s">
@@ -7665,16 +9808,16 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E76" s="9"/>
       <c r="F76" s="1" t="s">
@@ -7687,16 +9830,16 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="E77" s="9"/>
       <c r="F77" s="1" t="s">
@@ -7709,16 +9852,16 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="E78" s="9"/>
       <c r="F78" s="1" t="s">
@@ -7731,16 +9874,16 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="E79" s="9"/>
       <c r="F79" s="1" t="s">
@@ -7753,17 +9896,18 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>311</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="E80" s="9"/>
       <c r="F80" s="1" t="s">
         <v>153</v>
       </c>
@@ -7774,16 +9918,16 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="E81" s="9"/>
       <c r="F81" s="1" t="s">
@@ -7794,20 +9938,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="E82" s="9"/>
+        <v>311</v>
+      </c>
       <c r="F82" s="1" t="s">
         <v>153</v>
       </c>
@@ -7817,139 +9960,183 @@
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>320</v>
+      <c r="A83" s="11" t="s">
+        <v>312</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>58</v>
+        <v>314</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>322</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="E83" s="9"/>
       <c r="F83" s="1" t="s">
-        <v>323</v>
+        <v>153</v>
       </c>
       <c r="G83" s="7" t="b">
-        <f>TRUE</f>
-        <v>1</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="M83" s="1" t="s">
-        <v>324</v>
+        <f>FALSE</f>
+        <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>325</v>
+    <row r="84" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
+        <v>316</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>20</v>
+        <v>318</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>327</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="E84" s="9"/>
       <c r="F84" s="1" t="s">
-        <v>328</v>
+        <v>153</v>
       </c>
       <c r="G84" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>87</v>
+        <v>323</v>
       </c>
       <c r="G85" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="I85" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="K85" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="L85" s="13" t="s">
-        <v>468</v>
+        <v>92</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>87</v>
+        <v>328</v>
       </c>
       <c r="G86" s="7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>229</v>
+        <v>106</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>339</v>
+        <v>331</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>332</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G87" s="7" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
       <c r="H87" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="I87" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="L87" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G88" s="7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G89" s="7" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="H89" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="M87" s="1" t="s">
+      <c r="M89" s="1" t="s">
         <v>429</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M87" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:M89" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>

</xml_diff>